<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 10:48:54 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3875.6</v>
+        <v>3876.0</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>15.2</v>
+        <v>15.5</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -527,13 +527,13 @@
         <v/>
       </c>
       <c r="B4" t="str">
-        <v/>
+        <v>R4</v>
       </c>
       <c r="C4" t="str">
         <v/>
       </c>
       <c r="D4" t="str">
-        <v/>
+        <v>asq0342</v>
       </c>
       <c r="E4" t="str">
         <v/>
@@ -548,16 +548,16 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <v/>
+        <v>SCECO</v>
       </c>
       <c r="J4" t="str">
-        <v/>
+        <v>In progress</v>
       </c>
       <c r="K4" t="str">
         <v/>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>Latis</v>
       </c>
     </row>
   </sheetData>
@@ -1296,7 +1296,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>17.6</v>
+        <v>17.4</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>
@@ -1319,13 +1319,13 @@
         <v/>
       </c>
       <c r="B3" t="str">
-        <v>R4</v>
+        <v/>
       </c>
       <c r="C3" t="str">
         <v/>
       </c>
       <c r="D3" t="str">
-        <v>LTH0330</v>
+        <v/>
       </c>
       <c r="E3" t="str">
         <v/>
@@ -1340,16 +1340,16 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <v>SCECO+STB</v>
+        <v/>
       </c>
       <c r="J3" t="str">
-        <v>Good</v>
+        <v/>
       </c>
       <c r="K3" t="str">
         <v/>
       </c>
       <c r="L3" t="str">
-        <v>Latis</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 10:52:48 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3876.0</v>
+        <v>3876.1</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>15.5</v>
+        <v>15.7</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -533,7 +533,7 @@
         <v/>
       </c>
       <c r="D4" t="str">
-        <v>asq0342</v>
+        <v>JED0123</v>
       </c>
       <c r="E4" t="str">
         <v/>
@@ -560,9 +560,47 @@
         <v>Latis</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v>R4</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v>JED0123</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v>SCECO</v>
+      </c>
+      <c r="J5" t="str">
+        <v>In progress</v>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v>Latis</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 11:00:02 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3876.1</v>
+        <v>3876.0</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>15.7</v>
+        <v>15.5</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -533,7 +533,7 @@
         <v/>
       </c>
       <c r="D4" t="str">
-        <v>JED0123</v>
+        <v>LTH0330</v>
       </c>
       <c r="E4" t="str">
         <v/>
@@ -548,10 +548,10 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>SCECO</v>
+        <v>SCECO+STB</v>
       </c>
       <c r="J4" t="str">
-        <v>In progress</v>
+        <v>Good</v>
       </c>
       <c r="K4" t="str">
         <v/>
@@ -560,47 +560,9 @@
         <v>Latis</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v/>
-      </c>
-      <c r="B5" t="str">
-        <v>R4</v>
-      </c>
-      <c r="C5" t="str">
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <v>JED0123</v>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v>SCECO</v>
-      </c>
-      <c r="J5" t="str">
-        <v>In progress</v>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v>Latis</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 11:13:40 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -560,9 +560,47 @@
         <v>Latis</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v>R4</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v>JED0123</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v>SCECO</v>
+      </c>
+      <c r="J5" t="str">
+        <v>In progress</v>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v>Latis</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 11:15:25 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -571,7 +571,7 @@
         <v/>
       </c>
       <c r="D5" t="str">
-        <v>JED0123</v>
+        <v>JED0190</v>
       </c>
       <c r="E5" t="str">
         <v/>
@@ -589,7 +589,7 @@
         <v>SCECO</v>
       </c>
       <c r="J5" t="str">
-        <v>In progress</v>
+        <v>Good</v>
       </c>
       <c r="K5" t="str">
         <v/>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 11:33:39 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -598,9 +598,47 @@
         <v>Latis</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v>R4</v>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v>JED0123</v>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v>SCECO</v>
+      </c>
+      <c r="J6" t="str">
+        <v>In progress</v>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <v>Latis</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 11:38:31 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,9 +636,47 @@
         <v>Latis</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v>R4</v>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v>LTH2121</v>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <v>SCECO</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Dead</v>
+      </c>
+      <c r="K7" t="str">
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <v>Latis</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 11:47:56 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -527,7 +527,7 @@
         <v/>
       </c>
       <c r="B4" t="str">
-        <v>R4</v>
+        <v/>
       </c>
       <c r="C4" t="str">
         <v/>
@@ -548,135 +548,21 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>SCECO+STB</v>
+        <v/>
       </c>
       <c r="J4" t="str">
-        <v>Good</v>
+        <v/>
       </c>
       <c r="K4" t="str">
         <v/>
       </c>
       <c r="L4" t="str">
-        <v>Latis</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v/>
-      </c>
-      <c r="B5" t="str">
-        <v>R4</v>
-      </c>
-      <c r="C5" t="str">
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <v>JED0190</v>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v>SCECO</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Good</v>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v>Latis</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v/>
-      </c>
-      <c r="B6" t="str">
-        <v>R4</v>
-      </c>
-      <c r="C6" t="str">
-        <v/>
-      </c>
-      <c r="D6" t="str">
-        <v>JED0123</v>
-      </c>
-      <c r="E6" t="str">
-        <v/>
-      </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <v/>
-      </c>
-      <c r="H6" t="str">
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <v>SCECO</v>
-      </c>
-      <c r="J6" t="str">
-        <v>In progress</v>
-      </c>
-      <c r="K6" t="str">
-        <v/>
-      </c>
-      <c r="L6" t="str">
-        <v>Latis</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v/>
-      </c>
-      <c r="B7" t="str">
-        <v>R4</v>
-      </c>
-      <c r="C7" t="str">
-        <v/>
-      </c>
-      <c r="D7" t="str">
-        <v>LTH2121</v>
-      </c>
-      <c r="E7" t="str">
-        <v/>
-      </c>
-      <c r="F7" t="str">
-        <v/>
-      </c>
-      <c r="G7" t="str">
-        <v/>
-      </c>
-      <c r="H7" t="str">
-        <v/>
-      </c>
-      <c r="I7" t="str">
-        <v>SCECO</v>
-      </c>
-      <c r="J7" t="str">
-        <v>Dead</v>
-      </c>
-      <c r="K7" t="str">
-        <v/>
-      </c>
-      <c r="L7" t="str">
-        <v>Latis</v>
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 11:57:55 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -527,7 +527,7 @@
         <v/>
       </c>
       <c r="B4" t="str">
-        <v/>
+        <v>R4</v>
       </c>
       <c r="C4" t="str">
         <v/>
@@ -548,16 +548,16 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <v/>
+        <v>SCECO+STB</v>
       </c>
       <c r="J4" t="str">
-        <v/>
+        <v>Good</v>
       </c>
       <c r="K4" t="str">
         <v/>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>Latis</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 12:14:10 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -560,9 +560,47 @@
         <v>Latis</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v>R4</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v>JED0123</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v>SCECO</v>
+      </c>
+      <c r="J5" t="str">
+        <v>In progress</v>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v>Latis</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 5:42:22 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3876.0</v>
+        <v>3876:00:00</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>15.5</v>
+        <v>15:30:00</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -560,47 +560,9 @@
         <v>Latis</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v/>
-      </c>
-      <c r="B5" t="str">
-        <v>R4</v>
-      </c>
-      <c r="C5" t="str">
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <v>JED0123</v>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v>SCECO</v>
-      </c>
-      <c r="J5" t="str">
-        <v>In progress</v>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v>Latis</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -670,7 +632,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12057.0</v>
+        <v>12057:00:00</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -708,7 +670,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3186.7</v>
+        <v>3186:42:00</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -746,7 +708,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>424.9</v>
+        <v>424:54:00</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -964,7 +926,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2902.8</v>
+        <v>2902:48:00</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1002,7 +964,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>130.0</v>
+        <v>130:00:00</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1206,7 +1168,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>376.8</v>
+        <v>376:48:00</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1334,7 +1296,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>17.4</v>
+        <v>17:24:00</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 6:10:23 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3876:00:00</v>
+        <v>3883:24:06</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>15:30:00</v>
+        <v>22:56:44</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -632,7 +632,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12057:00:00</v>
+        <v>12064:47:47</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -670,7 +670,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3186:42:00</v>
+        <v>3194:31:16</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -708,7 +708,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>424:54:00</v>
+        <v>432:42:50</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -926,7 +926,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2902:48:00</v>
+        <v>2910:37:36</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -964,7 +964,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>130:00:00</v>
+        <v>137:49:51</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1168,7 +1168,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>376:48:00</v>
+        <v>384:36:35</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1296,7 +1296,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>17:24:00</v>
+        <v>25:08:53</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 6:18:20 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3883:24:06</v>
+        <v>3883:31:01</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>22:56:44</v>
+        <v>23:03:39</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -560,9 +560,47 @@
         <v>Latis</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -632,7 +670,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12064:47:47</v>
+        <v>12064:54:42</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -670,7 +708,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3194:31:16</v>
+        <v>3194:38:11</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -708,7 +746,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>432:42:50</v>
+        <v>432:49:45</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -926,7 +964,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2910:37:36</v>
+        <v>2910:44:31</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -964,7 +1002,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>137:49:51</v>
+        <v>137:56:46</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1168,7 +1206,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>384:36:35</v>
+        <v>384:43:30</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1296,7 +1334,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>25:08:53</v>
+        <v>25:15:48</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/16/2025, 6:22:52 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3883:31:01</v>
+        <v>3883:34:46</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>23:03:39</v>
+        <v>23:07:24</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -542,7 +542,7 @@
         <v/>
       </c>
       <c r="G4" t="str">
-        <v/>
+        <v>78679:13:57</v>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -670,7 +670,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12064:54:42</v>
+        <v>12064:58:27</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -708,7 +708,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3194:38:11</v>
+        <v>3194:41:56</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -746,7 +746,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>432:49:45</v>
+        <v>432:53:30</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -964,7 +964,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2910:44:31</v>
+        <v>2910:48:16</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1002,7 +1002,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>137:56:46</v>
+        <v>138:00:31</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1206,7 +1206,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>384:43:30</v>
+        <v>384:47:15</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1334,7 +1334,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>25:15:48</v>
+        <v>25:19:33</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:17:04 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3883:34:46</v>
+        <v>3918:31:03</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>23:07:24</v>
+        <v>58:03:41</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -542,7 +542,7 @@
         <v/>
       </c>
       <c r="G4" t="str">
-        <v>78679:13:57</v>
+        <v/>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -670,7 +670,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12064:58:27</v>
+        <v>12099:53:28</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -708,7 +708,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3194:41:56</v>
+        <v>3229:36:57</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -746,7 +746,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>432:53:30</v>
+        <v>467:48:31</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -964,7 +964,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2910:48:16</v>
+        <v>2945:43:17</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1002,7 +1002,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>138:00:31</v>
+        <v>172:55:32</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1206,7 +1206,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>384:47:15</v>
+        <v>419:42:16</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1334,7 +1334,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>25:19:33</v>
+        <v>60:14:34</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:21:41 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3918:31:03</v>
+        <v>3918:35:23</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>58:03:41</v>
+        <v>58:08:01</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -670,7 +670,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12099:53:28</v>
+        <v>12099:59:04</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -708,7 +708,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3229:36:57</v>
+        <v>3229:42:33</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -746,7 +746,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>467:48:31</v>
+        <v>467:54:07</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -964,7 +964,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2945:43:17</v>
+        <v>2945:48:53</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1002,7 +1002,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>172:55:32</v>
+        <v>173:01:08</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1206,7 +1206,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>419:42:16</v>
+        <v>419:47:52</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1334,7 +1334,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>60:14:34</v>
+        <v>60:20:10</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:22:05 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3918:35:23</v>
+        <v>3918:36:01</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>58:08:01</v>
+        <v>58:08:39</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -565,13 +565,13 @@
         <v/>
       </c>
       <c r="B5" t="str">
-        <v/>
+        <v>R4</v>
       </c>
       <c r="C5" t="str">
         <v/>
       </c>
       <c r="D5" t="str">
-        <v/>
+        <v>JED0123</v>
       </c>
       <c r="E5" t="str">
         <v/>
@@ -586,16 +586,16 @@
         <v/>
       </c>
       <c r="I5" t="str">
-        <v/>
+        <v>SCECO</v>
       </c>
       <c r="J5" t="str">
-        <v/>
+        <v>In progress</v>
       </c>
       <c r="K5" t="str">
         <v/>
       </c>
       <c r="L5" t="str">
-        <v/>
+        <v>Latis</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +670,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12099:59:04</v>
+        <v>12099:59:42</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -708,7 +708,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3229:42:33</v>
+        <v>3229:43:11</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -746,7 +746,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>467:54:07</v>
+        <v>467:54:45</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -964,7 +964,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2945:48:53</v>
+        <v>2945:49:31</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1002,7 +1002,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>173:01:08</v>
+        <v>173:01:46</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1206,7 +1206,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>419:47:52</v>
+        <v>419:48:30</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1334,7 +1334,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>60:20:10</v>
+        <v>60:20:48</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 9:12:37 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3918:36:01</v>
+        <v>3922:26:39</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>58:08:39</v>
+        <v>61:59:17</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -571,7 +571,7 @@
         <v/>
       </c>
       <c r="D5" t="str">
-        <v>JED0123</v>
+        <v>LTH2121</v>
       </c>
       <c r="E5" t="str">
         <v/>
@@ -589,7 +589,7 @@
         <v>SCECO</v>
       </c>
       <c r="J5" t="str">
-        <v>In progress</v>
+        <v>Dead</v>
       </c>
       <c r="K5" t="str">
         <v/>
@@ -670,7 +670,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12099:59:42</v>
+        <v>12103:50:20</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -708,7 +708,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3229:43:11</v>
+        <v>3233:33:49</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -746,7 +746,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>467:54:45</v>
+        <v>471:45:23</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -964,7 +964,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2945:49:31</v>
+        <v>2949:40:09</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1002,7 +1002,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>173:01:46</v>
+        <v>176:52:24</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1206,7 +1206,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>419:48:30</v>
+        <v>423:39:08</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1334,7 +1334,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>60:20:48</v>
+        <v>64:11:26</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 10:13:25 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3922:26:39</v>
+        <v>3923:27:31</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>61:59:17</v>
+        <v>63:00:09</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -598,9 +598,47 @@
         <v>Latis</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v>R4</v>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v>JED0123</v>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v>SCECO</v>
+      </c>
+      <c r="J6" t="str">
+        <v>In progress</v>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <v>Latis</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -670,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12103:50:20</v>
+        <v>12104:51:11</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -708,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3233:33:49</v>
+        <v>3234:34:40</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -746,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>471:45:23</v>
+        <v>472:46:14</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -964,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2949:40:09</v>
+        <v>2950:41:00</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1002,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>176:52:24</v>
+        <v>177:53:15</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1206,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>423:39:08</v>
+        <v>424:39:59</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1334,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>64:11:26</v>
+        <v>65:12:17</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 10:25:44 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3923:27:31</v>
+        <v>3923:39:59</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>63:00:09</v>
+        <v>63:12:37</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12104:51:11</v>
+        <v>12105:03:39</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3234:34:40</v>
+        <v>3234:47:08</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>472:46:14</v>
+        <v>472:58:42</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2950:41:00</v>
+        <v>2950:53:28</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>177:53:15</v>
+        <v>178:05:43</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>424:39:59</v>
+        <v>424:52:27</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>65:12:17</v>
+        <v>65:24:45</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 11:01:49 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3923:39:59</v>
+        <v>3924:15:59</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>63:12:37</v>
+        <v>63:48:37</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12105:03:39</v>
+        <v>12105:39:40</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3234:47:08</v>
+        <v>3235:23:09</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>472:58:42</v>
+        <v>473:34:43</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2950:53:28</v>
+        <v>2951:29:29</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>178:05:43</v>
+        <v>178:41:44</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>424:52:27</v>
+        <v>425:28:28</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>65:24:45</v>
+        <v>66:00:46</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 11:24:57 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3924:15:59</v>
+        <v>3924:39:11</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>63:48:37</v>
+        <v>64:11:49</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12105:39:40</v>
+        <v>12106:02:52</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3235:23:09</v>
+        <v>3235:46:21</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>473:34:43</v>
+        <v>473:57:55</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2951:29:29</v>
+        <v>2951:52:41</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>178:41:44</v>
+        <v>179:04:56</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>425:28:28</v>
+        <v>425:51:40</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>66:00:46</v>
+        <v>66:23:58</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 11:31:14 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3924:39:11</v>
+        <v>3924:45:23</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>64:11:49</v>
+        <v>64:18:01</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12106:02:52</v>
+        <v>12106:09:04</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3235:46:21</v>
+        <v>3235:52:33</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>473:57:55</v>
+        <v>474:04:07</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2951:52:41</v>
+        <v>2951:58:53</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>179:04:56</v>
+        <v>179:11:08</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>425:51:40</v>
+        <v>425:57:52</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>66:23:58</v>
+        <v>66:30:10</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 12:46:12 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3924:45:23</v>
+        <v>3926:00:22</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>64:18:01</v>
+        <v>65:33:00</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12106:09:04</v>
+        <v>12107:24:01</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3235:52:33</v>
+        <v>3237:07:30</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>474:04:07</v>
+        <v>475:19:04</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2951:58:53</v>
+        <v>2953:13:50</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>179:11:08</v>
+        <v>180:26:05</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>425:57:52</v>
+        <v>427:12:49</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>66:30:10</v>
+        <v>67:45:07</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 12:58:24 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:00:22</v>
+        <v>3926:12:40</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>65:33:00</v>
+        <v>65:45:18</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:24:01</v>
+        <v>12107:36:19</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:07:30</v>
+        <v>3237:19:48</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:19:04</v>
+        <v>475:31:22</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:13:50</v>
+        <v>2953:26:08</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:26:05</v>
+        <v>180:38:23</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:12:49</v>
+        <v>427:25:07</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>67:45:07</v>
+        <v>67:57:25</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 12:58:52 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:12:40</v>
+        <v>3926:13:07</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>65:45:18</v>
+        <v>65:45:45</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:36:19</v>
+        <v>12107:36:47</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:19:48</v>
+        <v>3237:20:16</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:31:22</v>
+        <v>475:31:50</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:26:08</v>
+        <v>2953:26:36</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:38:23</v>
+        <v>180:38:51</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:25:07</v>
+        <v>427:25:35</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>67:57:25</v>
+        <v>67:57:53</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 1:00:57 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:13:07</v>
+        <v>3926:15:11</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>65:45:45</v>
+        <v>65:47:49</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:36:47</v>
+        <v>12107:38:52</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:20:16</v>
+        <v>3237:22:21</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:31:50</v>
+        <v>475:33:55</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:26:36</v>
+        <v>2953:28:41</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:38:51</v>
+        <v>180:40:56</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:25:35</v>
+        <v>427:27:40</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>67:57:53</v>
+        <v>67:59:58</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 1:02:22 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:15:11</v>
+        <v>3926:16:37</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>65:47:49</v>
+        <v>65:49:15</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:38:52</v>
+        <v>12107:40:16</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:22:21</v>
+        <v>3237:23:45</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:33:55</v>
+        <v>475:35:19</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:28:41</v>
+        <v>2953:30:05</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:40:56</v>
+        <v>180:42:20</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:27:40</v>
+        <v>427:29:04</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>67:59:58</v>
+        <v>68:01:22</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 1:10:20 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:16:37</v>
+        <v>3926:24:33</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>65:49:15</v>
+        <v>65:57:11</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:40:16</v>
+        <v>12107:48:11</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:23:45</v>
+        <v>3237:31:40</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:35:19</v>
+        <v>475:43:14</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:30:05</v>
+        <v>2953:38:00</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:42:20</v>
+        <v>180:50:15</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:29:04</v>
+        <v>427:36:59</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>68:01:22</v>
+        <v>68:09:17</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 1:15:39 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:24:33</v>
+        <v>3926:29:43</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>65:57:11</v>
+        <v>66:02:21</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:48:11</v>
+        <v>12107:53:23</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:31:40</v>
+        <v>3237:36:52</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:43:14</v>
+        <v>475:48:26</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:38:00</v>
+        <v>2953:43:12</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:50:15</v>
+        <v>180:55:27</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:36:59</v>
+        <v>427:42:11</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>68:09:17</v>
+        <v>68:14:29</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 1:19:17 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:29:43</v>
+        <v>3926:33:31</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>66:02:21</v>
+        <v>66:06:09</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:53:23</v>
+        <v>12107:57:12</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:36:52</v>
+        <v>3237:40:41</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:48:26</v>
+        <v>475:52:15</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:43:12</v>
+        <v>2953:47:01</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:55:27</v>
+        <v>180:59:16</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:42:11</v>
+        <v>427:46:00</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>68:14:29</v>
+        <v>68:18:18</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 2:07:58 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -466,7 +466,7 @@
         <v>2025-01-05 22:45:44</v>
       </c>
       <c r="G2" t="str">
-        <v>3926:33:31</v>
+        <v>3927:21:57</v>
       </c>
       <c r="H2" t="str">
         <v>2025-01-05 22:38:30</v>
@@ -504,7 +504,7 @@
         <v>2025-06-15 19:13:06</v>
       </c>
       <c r="G3" t="str">
-        <v>66:06:09</v>
+        <v>66:54:35</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-15 19:13:06</v>
@@ -708,7 +708,7 @@
         <v>2024-01-31 01:22:03</v>
       </c>
       <c r="G2" t="str">
-        <v>12107:57:12</v>
+        <v>12108:45:38</v>
       </c>
       <c r="H2" t="str">
         <v>2024-01-31 01:13:03</v>
@@ -746,7 +746,7 @@
         <v>2025-02-03 15:38:34</v>
       </c>
       <c r="G3" t="str">
-        <v>3237:40:41</v>
+        <v>3238:29:07</v>
       </c>
       <c r="H3" t="str">
         <v>2025-02-03 15:30:04</v>
@@ -784,7 +784,7 @@
         <v>2025-05-29 17:27:00</v>
       </c>
       <c r="G4" t="str">
-        <v>475:52:15</v>
+        <v>476:40:41</v>
       </c>
       <c r="H4" t="str">
         <v>2025-05-14 13:02:01</v>
@@ -1002,7 +1002,7 @@
         <v>2025-02-15 11:32:14</v>
       </c>
       <c r="G2" t="str">
-        <v>2953:47:01</v>
+        <v>2954:35:27</v>
       </c>
       <c r="H2" t="str">
         <v>2025-02-15 11:23:40</v>
@@ -1040,7 +1040,7 @@
         <v>2025-06-11 00:19:59</v>
       </c>
       <c r="G3" t="str">
-        <v>180:59:16</v>
+        <v>181:47:42</v>
       </c>
       <c r="H3" t="str">
         <v>2025-06-10 22:04:05</v>
@@ -1244,7 +1244,7 @@
         <v>2025-05-31 17:33:15</v>
       </c>
       <c r="G2" t="str">
-        <v>427:46:00</v>
+        <v>428:34:26</v>
       </c>
       <c r="H2" t="str">
         <v>2025-05-30 17:59:05</v>
@@ -1372,7 +1372,7 @@
         <v>2025-06-15 17:00:57</v>
       </c>
       <c r="G2" t="str">
-        <v>68:18:18</v>
+        <v>69:06:44</v>
       </c>
       <c r="H2" t="str">
         <v>2025-06-15 17:18:01</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 2:14:02 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="94">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3927:27:54</t>
+    <t>3927:28:03</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>67:00:32</t>
+    <t>67:00:41</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -111,21 +111,12 @@
     <t>ETA 60 mins</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>LTH0330</t>
-  </si>
-  <si>
-    <t>SCECO+STB</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>LTH2121</t>
-  </si>
-  <si>
     <t>JED0123</t>
   </si>
   <si>
@@ -147,7 +138,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12108:51:35</t>
+    <t>12108:51:44</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -165,7 +156,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3238:35:04</t>
+    <t>3238:35:13</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -183,7 +174,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>476:46:38</t>
+    <t>476:46:47</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -204,7 +195,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2954:41:24</t>
+    <t>2954:41:33</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -222,7 +213,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>181:53:39</t>
+    <t>181:53:48</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -243,7 +234,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>70:06:04</t>
+    <t>70:06:13</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -258,7 +249,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>67:43:37</t>
+    <t>67:43:46</t>
   </si>
   <si>
     <t>25 m</t>
@@ -276,7 +267,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>428:40:23</t>
+    <t>428:40:32</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -300,7 +291,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>69:12:41</t>
+    <t>69:12:50</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -683,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -800,7 +791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -808,46 +799,33 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="K4" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="L4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -902,28 +880,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -932,7 +910,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -940,28 +918,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
         <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -970,7 +948,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -978,37 +956,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1114,28 +1092,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1144,7 +1122,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1152,28 +1130,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" t="s">
-        <v>69</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1182,7 +1160,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1190,31 +1168,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>72</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" t="s">
-        <v>76</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1222,31 +1200,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1303,28 +1281,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1333,7 +1311,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1341,7 +1319,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1395,28 +1373,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1425,7 +1403,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 2:34:54 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3927:28:03</t>
+    <t>3927:49:05</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>67:00:41</t>
+    <t>67:21:43</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -138,7 +138,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12108:51:44</t>
+    <t>12109:12:45</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -156,7 +156,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3238:35:13</t>
+    <t>3238:56:14</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -174,7 +174,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>476:46:47</t>
+    <t>477:07:48</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -195,7 +195,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2954:41:33</t>
+    <t>2955:02:34</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -213,7 +213,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>181:53:48</t>
+    <t>182:14:49</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -234,7 +234,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>70:06:13</t>
+    <t>70:27:14</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -249,7 +249,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>67:43:46</t>
+    <t>68:04:47</t>
   </si>
   <si>
     <t>25 m</t>
@@ -267,7 +267,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>428:40:32</t>
+    <t>429:01:33</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>69:12:50</t>
+    <t>69:33:51</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 3:33:14 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3927:49:05</t>
+    <t>3928:47:28</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>67:21:43</t>
+    <t>68:20:06</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -138,7 +138,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12109:12:45</t>
+    <t>12110:11:09</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -156,7 +156,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3238:56:14</t>
+    <t>3239:54:38</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -174,7 +174,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>477:07:48</t>
+    <t>478:06:12</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -195,7 +195,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2955:02:34</t>
+    <t>2956:00:58</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -213,7 +213,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>182:14:49</t>
+    <t>183:13:13</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -234,7 +234,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>70:27:14</t>
+    <t>71:25:38</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -249,7 +249,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>68:04:47</t>
+    <t>69:03:11</t>
   </si>
   <si>
     <t>25 m</t>
@@ -267,7 +267,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>429:01:33</t>
+    <t>429:59:57</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>69:33:51</t>
+    <t>70:32:15</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:26:11 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3928:47:28</t>
+    <t>3929:40:22</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>68:20:06</t>
+    <t>69:13:00</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -138,7 +138,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12110:11:09</t>
+    <t>12111:04:03</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -156,7 +156,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3239:54:38</t>
+    <t>3240:47:32</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -174,7 +174,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>478:06:12</t>
+    <t>478:59:06</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -195,7 +195,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:00:58</t>
+    <t>2956:53:52</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -213,7 +213,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>183:13:13</t>
+    <t>184:06:07</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -234,7 +234,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>71:25:38</t>
+    <t>72:18:32</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -249,7 +249,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:03:11</t>
+    <t>69:56:05</t>
   </si>
   <si>
     <t>25 m</t>
@@ -267,7 +267,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>429:59:57</t>
+    <t>430:52:51</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>70:32:15</t>
+    <t>71:25:09</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:28:06 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="94">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:40:22</t>
+    <t>3929:42:11</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:13:00</t>
+    <t>69:14:49</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -138,7 +138,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:04:03</t>
+    <t>12111:05:50</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -156,7 +156,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:47:32</t>
+    <t>3240:49:19</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -174,7 +174,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>478:59:06</t>
+    <t>479:00:53</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -195,7 +195,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:53:52</t>
+    <t>2956:55:39</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -213,7 +213,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:06:07</t>
+    <t>184:07:54</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -234,7 +234,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:18:32</t>
+    <t>72:20:19</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -249,7 +249,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:56:05</t>
+    <t>69:57:52</t>
   </si>
   <si>
     <t>25 m</t>
@@ -267,7 +267,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:52:51</t>
+    <t>430:54:38</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:25:09</t>
+    <t>71:26:56</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -674,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -826,6 +826,44 @@
         <v>31</v>
       </c>
       <c r="L4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:28:27 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:42:11</t>
+    <t>3929:42:41</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:14:49</t>
+    <t>69:15:19</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -138,7 +138,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:05:50</t>
+    <t>12111:06:10</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -156,7 +156,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:49:19</t>
+    <t>3240:49:39</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -174,7 +174,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:00:53</t>
+    <t>479:01:13</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -195,7 +195,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:55:39</t>
+    <t>2956:55:59</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -213,7 +213,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:07:54</t>
+    <t>184:08:14</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -234,7 +234,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:20:19</t>
+    <t>72:20:39</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -249,7 +249,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:57:52</t>
+    <t>69:58:12</t>
   </si>
   <si>
     <t>25 m</t>
@@ -267,7 +267,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:54:38</t>
+    <t>430:54:58</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:26:56</t>
+    <t>71:27:16</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:29:22 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="96">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:42:41</t>
+    <t>3929:43:11</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:15:19</t>
+    <t>69:15:49</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -123,6 +123,12 @@
     <t>In progress</t>
   </si>
   <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -138,7 +144,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:06:10</t>
+    <t>12111:06:27</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -156,7 +162,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:49:39</t>
+    <t>3240:49:56</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -174,7 +180,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:01:13</t>
+    <t>479:01:30</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -195,7 +201,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:55:59</t>
+    <t>2956:56:16</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -213,7 +219,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:08:14</t>
+    <t>184:08:31</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -234,7 +240,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:20:39</t>
+    <t>72:20:56</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -249,7 +255,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:58:12</t>
+    <t>69:58:29</t>
   </si>
   <si>
     <t>25 m</t>
@@ -267,7 +273,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:54:58</t>
+    <t>430:55:15</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -291,7 +297,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:27:16</t>
+    <t>71:27:33</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -840,7 +846,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -855,10 +861,10 @@
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -918,28 +924,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -948,7 +954,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -956,28 +962,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -986,7 +992,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -994,37 +1000,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1130,7 +1136,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1139,19 +1145,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1160,7 +1166,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1168,7 +1174,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1177,19 +1183,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1198,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1206,31 +1212,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1238,31 +1244,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1319,28 +1325,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1349,7 +1355,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1357,7 +1363,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1411,28 +1417,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1441,7 +1447,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:29:39 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:43:11</t>
+    <t>3929:43:47</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:15:49</t>
+    <t>69:16:25</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -144,7 +144,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:06:27</t>
+    <t>12111:07:28</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -162,7 +162,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:49:56</t>
+    <t>3240:50:57</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -180,7 +180,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:01:30</t>
+    <t>479:02:31</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -201,7 +201,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:56:16</t>
+    <t>2956:57:17</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -219,7 +219,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:08:31</t>
+    <t>184:09:32</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -240,7 +240,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:20:56</t>
+    <t>72:21:57</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -255,7 +255,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:58:29</t>
+    <t>69:59:30</t>
   </si>
   <si>
     <t>25 m</t>
@@ -273,7 +273,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:55:15</t>
+    <t>430:56:16</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -297,7 +297,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:27:33</t>
+    <t>71:28:34</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:29:49 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:43:47</t>
+    <t>3929:44:03</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:16:25</t>
+    <t>69:16:41</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -144,7 +144,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:07:28</t>
+    <t>12111:07:44</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -162,7 +162,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:50:57</t>
+    <t>3240:51:13</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -180,7 +180,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:02:31</t>
+    <t>479:02:47</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -201,7 +201,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:57:17</t>
+    <t>2956:57:33</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -219,7 +219,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:09:32</t>
+    <t>184:09:48</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -240,7 +240,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:21:57</t>
+    <t>72:22:13</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -255,7 +255,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:59:30</t>
+    <t>69:59:46</t>
   </si>
   <si>
     <t>25 m</t>
@@ -273,7 +273,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:56:16</t>
+    <t>430:56:32</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -297,7 +297,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:28:34</t>
+    <t>71:28:50</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:30:02 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:44:03</t>
+    <t>3929:44:15</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:16:41</t>
+    <t>69:16:53</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Good+In progress</t>
+  </si>
+  <si>
+    <t>LTH0330</t>
+  </si>
+  <si>
+    <t>SCECO+STB</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
   <si>
     <t>PCM-20250421-00001074</t>
@@ -680,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -870,6 +879,44 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -924,28 +971,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -954,7 +1001,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -962,28 +1009,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -992,7 +1039,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1000,37 +1047,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1136,7 +1183,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1145,19 +1192,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1166,7 +1213,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1174,7 +1221,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1183,19 +1230,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1204,7 +1251,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1212,31 +1259,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1244,31 +1291,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1325,28 +1372,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1355,7 +1402,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1363,7 +1410,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1417,28 +1464,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1447,7 +1494,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:30:06 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="96">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:44:15</t>
+    <t>3929:44:11</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:16:53</t>
+    <t>69:16:49</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -129,15 +129,6 @@
     <t>Good+In progress</t>
   </si>
   <si>
-    <t>LTH0330</t>
-  </si>
-  <si>
-    <t>SCECO+STB</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -153,7 +144,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:07:44</t>
+    <t>12111:07:45</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -171,7 +162,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:51:13</t>
+    <t>3240:51:14</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -189,7 +180,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:02:47</t>
+    <t>479:02:48</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -210,7 +201,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:57:33</t>
+    <t>2956:57:34</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -228,7 +219,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:09:48</t>
+    <t>184:09:49</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -249,7 +240,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:22:13</t>
+    <t>72:22:14</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -264,7 +255,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:59:46</t>
+    <t>69:59:47</t>
   </si>
   <si>
     <t>25 m</t>
@@ -282,7 +273,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:56:32</t>
+    <t>430:56:33</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -306,7 +297,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:28:50</t>
+    <t>71:28:51</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -689,7 +680,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -879,44 +870,6 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -971,28 +924,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1001,7 +954,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1009,28 +962,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1039,7 +992,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1047,37 +1000,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1183,7 +1136,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1192,19 +1145,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1213,7 +1166,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1221,7 +1174,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1230,19 +1183,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
         <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" t="s">
-        <v>71</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1251,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1259,31 +1212,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
         <v>74</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1291,31 +1244,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1372,28 +1325,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1402,7 +1355,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1410,7 +1363,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1464,28 +1417,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1494,7 +1447,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:30:43 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:44:11</t>
+    <t>3929:44:38</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:16:49</t>
+    <t>69:17:16</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -129,6 +129,15 @@
     <t>Good+In progress</t>
   </si>
   <si>
+    <t>LTH0330</t>
+  </si>
+  <si>
+    <t>SCECO+STB</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -144,7 +153,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:07:45</t>
+    <t>12111:08:19</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -162,7 +171,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:51:14</t>
+    <t>3240:51:48</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -180,7 +189,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:02:48</t>
+    <t>479:03:22</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -201,7 +210,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:57:34</t>
+    <t>2956:58:08</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -219,7 +228,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:09:49</t>
+    <t>184:10:23</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -240,7 +249,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:22:14</t>
+    <t>72:22:48</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -255,7 +264,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>69:59:47</t>
+    <t>70:00:21</t>
   </si>
   <si>
     <t>25 m</t>
@@ -273,7 +282,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:56:33</t>
+    <t>430:57:07</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -297,7 +306,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:28:51</t>
+    <t>71:29:25</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -680,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -870,6 +879,44 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -924,28 +971,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -954,7 +1001,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -962,28 +1009,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -992,7 +1039,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1000,37 +1047,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1136,7 +1183,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1145,19 +1192,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1166,7 +1213,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1174,7 +1221,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1183,19 +1230,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1204,7 +1251,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1212,31 +1259,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1244,31 +1291,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1325,28 +1372,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1355,7 +1402,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1363,7 +1410,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1417,28 +1464,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1447,7 +1494,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:32:04 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="100">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:44:38</t>
+    <t>3929:45:14</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:17:16</t>
+    <t>69:17:52</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -129,15 +129,6 @@
     <t>Good+In progress</t>
   </si>
   <si>
-    <t>LTH0330</t>
-  </si>
-  <si>
-    <t>SCECO+STB</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -153,7 +144,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:08:19</t>
+    <t>12111:08:55</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -171,7 +162,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:51:48</t>
+    <t>3240:52:24</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -189,7 +180,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:03:22</t>
+    <t>479:03:58</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -201,6 +192,18 @@
     <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
   </si>
   <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>HAL0947</t>
+  </si>
+  <si>
+    <t>Weak+Good</t>
+  </si>
+  <si>
+    <t>Zain</t>
+  </si>
+  <si>
     <t xml:space="preserve"> PCM-20250215-00000830 </t>
   </si>
   <si>
@@ -210,7 +213,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:58:08</t>
+    <t>2956:58:44</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -228,7 +231,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:10:23</t>
+    <t>184:10:59</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -249,7 +252,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:22:48</t>
+    <t>72:23:24</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -264,7 +267,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:00:21</t>
+    <t>70:00:57</t>
   </si>
   <si>
     <t>25 m</t>
@@ -282,7 +285,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:57:07</t>
+    <t>430:57:43</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -306,7 +309,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:29:25</t>
+    <t>71:30:01</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -689,7 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -879,44 +882,6 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -971,28 +936,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1001,7 +966,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1009,28 +974,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1039,7 +1004,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1047,37 +1012,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1091,7 +1056,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1130,6 +1095,44 @@
       </c>
       <c r="L1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1183,7 +1186,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1192,19 +1195,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1213,7 +1216,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1221,7 +1224,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1230,19 +1233,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1251,7 +1254,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1259,31 +1262,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1291,31 +1294,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1372,28 +1375,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1402,7 +1405,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1410,7 +1413,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1464,28 +1467,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1494,7 +1497,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:32:49 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="97">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:45:14</t>
+    <t>3929:46:41</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:17:52</t>
+    <t>69:19:19</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -111,150 +111,141 @@
     <t>ETA 60 mins</t>
   </si>
   <si>
+    <t>PCM-20250421-00001074</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RIY2486</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>12111:10:08</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:13:03</t>
+  </si>
+  <si>
+    <t>site located in VIP Area and Generator switched off as per security request.</t>
+  </si>
+  <si>
+    <t>PCM-20250203-00001501</t>
+  </si>
+  <si>
+    <t>RIY2719</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:38:34</t>
+  </si>
+  <si>
+    <t>3240:53:37</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:30:04</t>
+  </si>
+  <si>
+    <t>Access Issue As Site located inside Wonder Garden.</t>
+  </si>
+  <si>
+    <t>PCM-20250529-00002138</t>
+  </si>
+  <si>
+    <t>RIY2903</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:27:00</t>
+  </si>
+  <si>
+    <t>479:05:11</t>
+  </si>
+  <si>
+    <t>2025-05-14 13:02:01</t>
+  </si>
+  <si>
+    <t>No BB</t>
+  </si>
+  <si>
+    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>HAL0947</t>
+  </si>
+  <si>
+    <t>Weak+Good</t>
+  </si>
+  <si>
+    <t>Zain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCM-20250215-00000830 </t>
+  </si>
+  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>JED0123</t>
+    <t>MKJD0649</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:32:14</t>
+  </si>
+  <si>
+    <t>2956:59:57</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:23:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
+  </si>
+  <si>
+    <t>PCM-20250611-00000037</t>
+  </si>
+  <si>
+    <t>JED2394</t>
+  </si>
+  <si>
+    <t>2025-06-11 00:19:59</t>
+  </si>
+  <si>
+    <t>184:12:12</t>
+  </si>
+  <si>
+    <t>2025-06-10 22:04:05</t>
+  </si>
+  <si>
+    <t>Site access issue  located in formula one  /Site under relocation</t>
+  </si>
+  <si>
+    <t>NO PCM</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TAF0156</t>
+  </si>
+  <si>
+    <t>2025-06-15 16:07:34</t>
+  </si>
+  <si>
+    <t>72:24:37</t>
   </si>
   <si>
     <t>In progress</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
-  </si>
-  <si>
-    <t>PCM-20250421-00001074</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RIY2486</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>12111:08:55</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:13:03</t>
-  </si>
-  <si>
-    <t>site located in VIP Area and Generator switched off as per security request.</t>
-  </si>
-  <si>
-    <t>PCM-20250203-00001501</t>
-  </si>
-  <si>
-    <t>RIY2719</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:38:34</t>
-  </si>
-  <si>
-    <t>3240:52:24</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:30:04</t>
-  </si>
-  <si>
-    <t>Access Issue As Site located inside Wonder Garden.</t>
-  </si>
-  <si>
-    <t>PCM-20250529-00002138</t>
-  </si>
-  <si>
-    <t>RIY2903</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:27:00</t>
-  </si>
-  <si>
-    <t>479:03:58</t>
-  </si>
-  <si>
-    <t>2025-05-14 13:02:01</t>
-  </si>
-  <si>
-    <t>No BB</t>
-  </si>
-  <si>
-    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>HAL0947</t>
-  </si>
-  <si>
-    <t>Weak+Good</t>
-  </si>
-  <si>
-    <t>Zain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PCM-20250215-00000830 </t>
-  </si>
-  <si>
-    <t>MKJD0649</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:32:14</t>
-  </si>
-  <si>
-    <t>2956:58:44</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:23:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
-  </si>
-  <si>
-    <t>PCM-20250611-00000037</t>
-  </si>
-  <si>
-    <t>JED2394</t>
-  </si>
-  <si>
-    <t>2025-06-11 00:19:59</t>
-  </si>
-  <si>
-    <t>184:10:59</t>
-  </si>
-  <si>
-    <t>2025-06-10 22:04:05</t>
-  </si>
-  <si>
-    <t>Site access issue  located in formula one  /Site under relocation</t>
-  </si>
-  <si>
-    <t>NO PCM</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>TAF0156</t>
-  </si>
-  <si>
-    <t>2025-06-15 16:07:34</t>
-  </si>
-  <si>
-    <t>72:23:24</t>
-  </si>
-  <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
   </si>
   <si>
@@ -267,7 +258,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:00:57</t>
+    <t>70:02:10</t>
   </si>
   <si>
     <t>25 m</t>
@@ -285,7 +276,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:57:43</t>
+    <t>430:58:56</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -309,7 +300,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:30:01</t>
+    <t>71:31:14</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -692,7 +683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -806,82 +797,6 @@
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -936,28 +851,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -966,7 +881,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -974,28 +889,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1004,7 +919,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1012,37 +927,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1099,40 +1014,40 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1186,28 +1101,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1216,7 +1131,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1224,28 +1139,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1254,7 +1169,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1262,31 +1177,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
         <v>76</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>79</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1294,31 +1209,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1375,28 +1290,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1405,7 +1320,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1413,7 +1328,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1467,28 +1382,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1497,7 +1412,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:33:42 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="100">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:46:41</t>
+    <t>3929:47:41</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:19:19</t>
+    <t>69:20:19</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -111,6 +111,33 @@
     <t>ETA 60 mins</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>JED0123</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -120,13 +147,7 @@
     <t>RIY2486</t>
   </si>
   <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>12111:10:08</t>
+    <t>12111:11:08</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -144,7 +165,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:53:37</t>
+    <t>3240:54:37</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -162,7 +183,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:05:11</t>
+    <t>479:06:11</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -174,9 +195,6 @@
     <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -192,16 +210,13 @@
     <t xml:space="preserve"> PCM-20250215-00000830 </t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>MKJD0649</t>
   </si>
   <si>
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2956:59:57</t>
+    <t>2957:00:57</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -219,7 +234,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:12:12</t>
+    <t>184:13:12</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -240,25 +255,19 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:24:37</t>
-  </si>
-  <si>
-    <t>In progress</t>
+    <t>72:25:37</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>JED0674</t>
   </si>
   <si>
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:02:10</t>
+    <t>70:03:10</t>
   </si>
   <si>
     <t>25 m</t>
@@ -276,7 +285,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:58:56</t>
+    <t>430:59:56</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -300,7 +309,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:31:14</t>
+    <t>71:32:14</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -683,7 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -797,6 +806,82 @@
         <v>30</v>
       </c>
       <c r="L3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -851,28 +936,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -881,7 +966,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -889,28 +974,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -919,7 +1004,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -927,37 +1012,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1014,40 +1099,40 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1101,28 +1186,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1131,7 +1216,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1139,28 +1224,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1169,7 +1254,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1177,31 +1262,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" t="s">
-        <v>75</v>
-      </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1209,31 +1294,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1290,28 +1375,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1320,7 +1405,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1328,7 +1413,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1382,28 +1467,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1412,7 +1497,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:33:45 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:47:41</t>
+    <t>3929:47:52</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:20:19</t>
+    <t>69:20:30</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -117,157 +117,154 @@
     <t>R4</t>
   </si>
   <si>
-    <t>JED0123</t>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
+    <t>PCM-20250421-00001074</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RIY2486</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>12111:11:30</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:13:03</t>
+  </si>
+  <si>
+    <t>site located in VIP Area and Generator switched off as per security request.</t>
+  </si>
+  <si>
+    <t>PCM-20250203-00001501</t>
+  </si>
+  <si>
+    <t>RIY2719</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:38:34</t>
+  </si>
+  <si>
+    <t>3240:54:59</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:30:04</t>
+  </si>
+  <si>
+    <t>Access Issue As Site located inside Wonder Garden.</t>
+  </si>
+  <si>
+    <t>PCM-20250529-00002138</t>
+  </si>
+  <si>
+    <t>RIY2903</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:27:00</t>
+  </si>
+  <si>
+    <t>479:06:33</t>
+  </si>
+  <si>
+    <t>2025-05-14 13:02:01</t>
+  </si>
+  <si>
+    <t>No BB</t>
+  </si>
+  <si>
+    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>HAL0947</t>
+  </si>
+  <si>
+    <t>Weak+Good</t>
+  </si>
+  <si>
+    <t>Zain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCM-20250215-00000830 </t>
+  </si>
+  <si>
+    <t>MKJD0649</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:32:14</t>
+  </si>
+  <si>
+    <t>2957:01:19</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:23:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
+  </si>
+  <si>
+    <t>PCM-20250611-00000037</t>
+  </si>
+  <si>
+    <t>JED2394</t>
+  </si>
+  <si>
+    <t>2025-06-11 00:19:59</t>
+  </si>
+  <si>
+    <t>184:13:34</t>
+  </si>
+  <si>
+    <t>2025-06-10 22:04:05</t>
+  </si>
+  <si>
+    <t>Site access issue  located in formula one  /Site under relocation</t>
+  </si>
+  <si>
+    <t>NO PCM</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TAF0156</t>
+  </si>
+  <si>
+    <t>2025-06-15 16:07:34</t>
+  </si>
+  <si>
+    <t>72:25:59</t>
   </si>
   <si>
     <t>In progress</t>
   </si>
   <si>
+    <t>Access issue, located on commercial building, due to pending rent billing</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
-  </si>
-  <si>
-    <t>PCM-20250421-00001074</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RIY2486</t>
-  </si>
-  <si>
-    <t>12111:11:08</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:13:03</t>
-  </si>
-  <si>
-    <t>site located in VIP Area and Generator switched off as per security request.</t>
-  </si>
-  <si>
-    <t>PCM-20250203-00001501</t>
-  </si>
-  <si>
-    <t>RIY2719</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:38:34</t>
-  </si>
-  <si>
-    <t>3240:54:37</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:30:04</t>
-  </si>
-  <si>
-    <t>Access Issue As Site located inside Wonder Garden.</t>
-  </si>
-  <si>
-    <t>PCM-20250529-00002138</t>
-  </si>
-  <si>
-    <t>RIY2903</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:27:00</t>
-  </si>
-  <si>
-    <t>479:06:11</t>
-  </si>
-  <si>
-    <t>2025-05-14 13:02:01</t>
-  </si>
-  <si>
-    <t>No BB</t>
-  </si>
-  <si>
-    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>HAL0947</t>
-  </si>
-  <si>
-    <t>Weak+Good</t>
-  </si>
-  <si>
-    <t>Zain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PCM-20250215-00000830 </t>
-  </si>
-  <si>
-    <t>MKJD0649</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:32:14</t>
-  </si>
-  <si>
-    <t>2957:00:57</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:23:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
-  </si>
-  <si>
-    <t>PCM-20250611-00000037</t>
-  </si>
-  <si>
-    <t>JED2394</t>
-  </si>
-  <si>
-    <t>2025-06-11 00:19:59</t>
-  </si>
-  <si>
-    <t>184:13:12</t>
-  </si>
-  <si>
-    <t>2025-06-10 22:04:05</t>
-  </si>
-  <si>
-    <t>Site access issue  located in formula one  /Site under relocation</t>
-  </si>
-  <si>
-    <t>NO PCM</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>TAF0156</t>
-  </si>
-  <si>
-    <t>2025-06-15 16:07:34</t>
-  </si>
-  <si>
-    <t>72:25:37</t>
-  </si>
-  <si>
-    <t>Access issue, located on commercial building, due to pending rent billing</t>
-  </si>
-  <si>
     <t>JED0674</t>
   </si>
   <si>
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:03:10</t>
+    <t>70:03:32</t>
   </si>
   <si>
     <t>25 m</t>
@@ -285,7 +282,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>430:59:56</t>
+    <t>431:00:18</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -309,7 +306,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:32:14</t>
+    <t>71:32:36</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -692,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -835,7 +832,7 @@
         <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
         <v>34</v>
@@ -844,44 +841,6 @@
         <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -936,28 +895,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -966,7 +925,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -974,28 +933,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
         <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1004,7 +963,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1012,37 +971,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1102,13 +1061,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1126,13 +1085,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1186,7 +1145,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1195,19 +1154,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1216,7 +1175,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1224,7 +1183,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1233,19 +1192,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
         <v>70</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" t="s">
-        <v>73</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1254,7 +1213,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1262,31 +1221,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
         <v>76</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>77</v>
       </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>78</v>
-      </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>80</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1294,31 +1253,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
         <v>82</v>
-      </c>
-      <c r="G5" t="s">
-        <v>83</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1375,28 +1334,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" t="s">
-        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>89</v>
-      </c>
-      <c r="H2" t="s">
-        <v>90</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1405,7 +1364,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1413,7 +1372,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1467,28 +1426,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
         <v>96</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>97</v>
-      </c>
-      <c r="H2" t="s">
-        <v>98</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1497,7 +1456,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:35:15 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="101">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:47:52</t>
+    <t>3929:49:11</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:20:30</t>
+    <t>69:21:49</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -117,10 +117,22 @@
     <t>R4</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
+    <t>JED0925</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>2025-06-14 20:13:06</t>
+  </si>
+  <si>
+    <t>93:21:49</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>team on the way</t>
   </si>
   <si>
     <t>PCM-20250421-00001074</t>
@@ -132,13 +144,10 @@
     <t>RIY2486</t>
   </si>
   <si>
-    <t>Critical</t>
-  </si>
-  <si>
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:11:30</t>
+    <t>12111:12:24</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -156,7 +165,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:54:59</t>
+    <t>3240:55:53</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -174,7 +183,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:06:33</t>
+    <t>479:07:27</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -207,7 +216,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:01:19</t>
+    <t>2957:02:13</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -225,7 +234,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:13:34</t>
+    <t>184:14:28</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -246,10 +255,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:25:59</t>
-  </si>
-  <si>
-    <t>In progress</t>
+    <t>72:26:53</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -264,7 +270,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:03:32</t>
+    <t>70:04:26</t>
   </si>
   <si>
     <t>25 m</t>
@@ -282,7 +288,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:00:18</t>
+    <t>431:01:12</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -306,7 +312,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:32:36</t>
+    <t>71:33:30</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -814,19 +820,19 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -835,10 +841,10 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -895,28 +901,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -925,7 +931,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -933,28 +939,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -963,7 +969,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -971,37 +977,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1061,13 +1067,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1085,13 +1091,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1151,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1154,19 +1160,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1175,7 +1181,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1183,7 +1189,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1192,19 +1198,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1213,7 +1219,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1221,31 +1227,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1253,31 +1259,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1334,28 +1340,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1364,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1372,7 +1378,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1426,28 +1432,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1456,7 +1462,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:50:25 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="103">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3929:49:11</t>
+    <t>3930:04:24</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:21:49</t>
+    <t>69:37:02</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>93:21:49</t>
+    <t>92:37:02</t>
   </si>
   <si>
     <t>In progress</t>
@@ -135,6 +135,12 @@
     <t>team on the way</t>
   </si>
   <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -147,7 +153,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:12:24</t>
+    <t>12111:28:05</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -165,7 +171,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3240:55:53</t>
+    <t>3241:11:34</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -183,7 +189,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:07:27</t>
+    <t>479:23:08</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -216,7 +222,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:02:13</t>
+    <t>2957:17:54</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -234,7 +240,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:14:28</t>
+    <t>184:30:09</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -255,7 +261,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:26:53</t>
+    <t>72:42:34</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -270,7 +276,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:04:26</t>
+    <t>70:20:07</t>
   </si>
   <si>
     <t>25 m</t>
@@ -288,7 +294,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:01:12</t>
+    <t>431:16:53</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -312,7 +318,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:33:30</t>
+    <t>71:49:11</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -695,7 +701,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -847,6 +853,44 @@
         <v>38</v>
       </c>
       <c r="L4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -901,28 +945,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -931,7 +975,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -939,28 +983,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -969,7 +1013,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -977,37 +1021,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1067,13 +1111,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1091,13 +1135,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1195,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1160,19 +1204,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1181,7 +1225,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1189,7 +1233,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1198,19 +1242,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1219,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1227,31 +1271,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1259,31 +1303,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1340,28 +1384,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1370,7 +1414,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1378,7 +1422,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1432,28 +1476,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1462,7 +1506,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 4:58:32 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:04:24</t>
+    <t>3930:12:23</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:37:02</t>
+    <t>69:45:01</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:37:02</t>
+    <t>92:45:01</t>
   </si>
   <si>
     <t>In progress</t>
@@ -135,10 +135,13 @@
     <t>team on the way</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>HAJ0155</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
   <si>
     <t>PCM-20250421-00001074</t>
@@ -153,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:28:05</t>
+    <t>12111:36:04</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -171,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3241:11:34</t>
+    <t>3241:19:33</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -189,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:23:08</t>
+    <t>479:31:07</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -222,7 +225,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:17:54</t>
+    <t>2957:25:53</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -240,7 +243,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:30:09</t>
+    <t>184:38:08</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -261,7 +264,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:42:34</t>
+    <t>72:50:33</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -276,7 +279,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:20:07</t>
+    <t>70:28:06</t>
   </si>
   <si>
     <t>25 m</t>
@@ -285,16 +288,13 @@
     <t>PCM-20250531-00001907</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>MAK0605</t>
   </si>
   <si>
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:16:53</t>
+    <t>431:24:52</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -318,7 +318,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:49:11</t>
+    <t>71:57:10</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -861,13 +861,13 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -882,10 +882,10 @@
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -945,28 +945,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -975,7 +975,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -983,28 +983,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1013,7 +1013,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1021,37 +1021,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1111,13 +1111,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1135,13 +1135,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1204,19 +1204,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1225,7 +1225,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1242,19 +1242,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1263,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1271,31 +1271,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1303,31 +1303,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1384,10 +1384,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:00:06 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:12:23</t>
+    <t>3930:14:12</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:45:01</t>
+    <t>69:46:50</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:45:01</t>
+    <t>92:46:50</t>
   </si>
   <si>
     <t>In progress</t>
@@ -135,166 +135,166 @@
     <t>team on the way</t>
   </si>
   <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
+    <t>PCM-20250421-00001074</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RIY2486</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>12111:37:53</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:13:03</t>
+  </si>
+  <si>
+    <t>site located in VIP Area and Generator switched off as per security request.</t>
+  </si>
+  <si>
+    <t>PCM-20250203-00001501</t>
+  </si>
+  <si>
+    <t>RIY2719</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:38:34</t>
+  </si>
+  <si>
+    <t>3241:21:22</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:30:04</t>
+  </si>
+  <si>
+    <t>Access Issue As Site located inside Wonder Garden.</t>
+  </si>
+  <si>
+    <t>PCM-20250529-00002138</t>
+  </si>
+  <si>
+    <t>RIY2903</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:27:00</t>
+  </si>
+  <si>
+    <t>479:32:56</t>
+  </si>
+  <si>
+    <t>2025-05-14 13:02:01</t>
+  </si>
+  <si>
+    <t>No BB</t>
+  </si>
+  <si>
+    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>HAL0947</t>
+  </si>
+  <si>
+    <t>Weak+Good</t>
+  </si>
+  <si>
+    <t>Zain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCM-20250215-00000830 </t>
+  </si>
+  <si>
+    <t>MKJD0649</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:32:14</t>
+  </si>
+  <si>
+    <t>2957:27:42</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:23:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
+  </si>
+  <si>
+    <t>PCM-20250611-00000037</t>
+  </si>
+  <si>
+    <t>JED2394</t>
+  </si>
+  <si>
+    <t>2025-06-11 00:19:59</t>
+  </si>
+  <si>
+    <t>184:39:57</t>
+  </si>
+  <si>
+    <t>2025-06-10 22:04:05</t>
+  </si>
+  <si>
+    <t>Site access issue  located in formula one  /Site under relocation</t>
+  </si>
+  <si>
+    <t>NO PCM</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TAF0156</t>
+  </si>
+  <si>
+    <t>2025-06-15 16:07:34</t>
+  </si>
+  <si>
+    <t>72:52:22</t>
+  </si>
+  <si>
+    <t>Access issue, located on commercial building, due to pending rent billing</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>JED0674</t>
+  </si>
+  <si>
+    <t>2025-06-15 18:30:01</t>
+  </si>
+  <si>
+    <t>70:29:55</t>
+  </si>
+  <si>
+    <t>25 m</t>
+  </si>
+  <si>
+    <t>PCM-20250531-00001907</t>
+  </si>
+  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>HAJ0155</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>PCM-20250421-00001074</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RIY2486</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>12111:36:04</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:13:03</t>
-  </si>
-  <si>
-    <t>site located in VIP Area and Generator switched off as per security request.</t>
-  </si>
-  <si>
-    <t>PCM-20250203-00001501</t>
-  </si>
-  <si>
-    <t>RIY2719</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:38:34</t>
-  </si>
-  <si>
-    <t>3241:19:33</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:30:04</t>
-  </si>
-  <si>
-    <t>Access Issue As Site located inside Wonder Garden.</t>
-  </si>
-  <si>
-    <t>PCM-20250529-00002138</t>
-  </si>
-  <si>
-    <t>RIY2903</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:27:00</t>
-  </si>
-  <si>
-    <t>479:31:07</t>
-  </si>
-  <si>
-    <t>2025-05-14 13:02:01</t>
-  </si>
-  <si>
-    <t>No BB</t>
-  </si>
-  <si>
-    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>HAL0947</t>
-  </si>
-  <si>
-    <t>Weak+Good</t>
-  </si>
-  <si>
-    <t>Zain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PCM-20250215-00000830 </t>
-  </si>
-  <si>
-    <t>MKJD0649</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:32:14</t>
-  </si>
-  <si>
-    <t>2957:25:53</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:23:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
-  </si>
-  <si>
-    <t>PCM-20250611-00000037</t>
-  </si>
-  <si>
-    <t>JED2394</t>
-  </si>
-  <si>
-    <t>2025-06-11 00:19:59</t>
-  </si>
-  <si>
-    <t>184:38:08</t>
-  </si>
-  <si>
-    <t>2025-06-10 22:04:05</t>
-  </si>
-  <si>
-    <t>Site access issue  located in formula one  /Site under relocation</t>
-  </si>
-  <si>
-    <t>NO PCM</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>TAF0156</t>
-  </si>
-  <si>
-    <t>2025-06-15 16:07:34</t>
-  </si>
-  <si>
-    <t>72:50:33</t>
-  </si>
-  <si>
-    <t>Access issue, located on commercial building, due to pending rent billing</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>JED0674</t>
-  </si>
-  <si>
-    <t>2025-06-15 18:30:01</t>
-  </si>
-  <si>
-    <t>70:28:06</t>
-  </si>
-  <si>
-    <t>25 m</t>
-  </si>
-  <si>
-    <t>PCM-20250531-00001907</t>
-  </si>
-  <si>
     <t>MAK0605</t>
   </si>
   <si>
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:24:52</t>
+    <t>431:26:41</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -318,7 +318,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:57:10</t>
+    <t>71:58:59</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -861,13 +861,13 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -882,10 +882,10 @@
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -945,28 +945,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -975,7 +975,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -983,28 +983,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
         <v>51</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1013,7 +1013,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1021,37 +1021,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
         <v>57</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>58</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" t="s">
         <v>60</v>
-      </c>
-      <c r="K4" t="s">
-        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1111,13 +1111,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1135,13 +1135,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1204,19 +1204,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>69</v>
-      </c>
-      <c r="H2" t="s">
-        <v>70</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1225,7 +1225,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1242,19 +1242,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>75</v>
-      </c>
-      <c r="H3" t="s">
-        <v>76</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1263,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1271,31 +1271,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
         <v>79</v>
-      </c>
-      <c r="D4" t="s">
-        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
         <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>82</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1303,31 +1303,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
-      </c>
-      <c r="D5" t="s">
-        <v>85</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
         <v>86</v>
-      </c>
-      <c r="G5" t="s">
-        <v>87</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1384,10 +1384,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:00:57 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:14:12</t>
+    <t>3930:15:01</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:46:50</t>
+    <t>69:47:39</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:46:50</t>
+    <t>92:47:39</t>
   </si>
   <si>
     <t>In progress</t>
@@ -135,10 +135,13 @@
     <t>team on the way</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>HAJ0155</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
   <si>
     <t>PCM-20250421-00001074</t>
@@ -153,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:37:53</t>
+    <t>12111:38:28</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -171,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3241:21:22</t>
+    <t>3241:21:57</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -189,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:32:56</t>
+    <t>479:33:31</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -213,6 +216,12 @@
     <t>Zain</t>
   </si>
   <si>
+    <t>HAJ0125</t>
+  </si>
+  <si>
+    <t>Haj Removal</t>
+  </si>
+  <si>
     <t xml:space="preserve"> PCM-20250215-00000830 </t>
   </si>
   <si>
@@ -222,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:27:42</t>
+    <t>2957:28:17</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -240,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:39:57</t>
+    <t>184:40:32</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -261,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:52:22</t>
+    <t>72:52:57</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -276,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:29:55</t>
+    <t>70:30:30</t>
   </si>
   <si>
     <t>25 m</t>
@@ -285,16 +294,13 @@
     <t>PCM-20250531-00001907</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>MAK0605</t>
   </si>
   <si>
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:26:41</t>
+    <t>431:27:16</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -318,7 +324,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:58:59</t>
+    <t>71:59:34</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -861,13 +867,13 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -882,10 +888,10 @@
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -945,28 +951,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -975,7 +981,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -983,28 +989,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1013,7 +1019,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1021,37 +1027,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1065,7 +1071,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1111,13 +1117,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1135,13 +1141,51 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1239,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1204,19 +1248,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1225,7 +1269,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1233,7 +1277,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1242,19 +1286,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1263,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1271,31 +1315,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1303,31 +1347,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1384,28 +1428,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1414,7 +1458,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1422,7 +1466,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1476,28 +1520,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1506,7 +1550,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:01:43 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="102">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:15:01</t>
+    <t>3930:15:41</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:47:39</t>
+    <t>69:48:19</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:47:39</t>
+    <t>92:48:19</t>
   </si>
   <si>
     <t>In progress</t>
@@ -156,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:38:28</t>
+    <t>12111:39:21</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3241:21:57</t>
+    <t>3241:22:50</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:33:31</t>
+    <t>479:34:24</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -216,12 +216,6 @@
     <t>Zain</t>
   </si>
   <si>
-    <t>HAJ0125</t>
-  </si>
-  <si>
-    <t>Haj Removal</t>
-  </si>
-  <si>
     <t xml:space="preserve"> PCM-20250215-00000830 </t>
   </si>
   <si>
@@ -231,7 +225,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:28:17</t>
+    <t>2957:29:10</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -249,7 +243,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:40:32</t>
+    <t>184:41:25</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -270,7 +264,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:52:57</t>
+    <t>72:53:50</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -285,7 +279,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:30:30</t>
+    <t>70:31:23</t>
   </si>
   <si>
     <t>25 m</t>
@@ -300,7 +294,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:27:16</t>
+    <t>431:28:09</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -309,9 +303,6 @@
     <t>Sectors are down due to TE issue and they are facing access issue. Access applied and waiting approval from court.</t>
   </si>
   <si>
-    <t>MAK0875</t>
-  </si>
-  <si>
     <t>PCM-20250615-00001771</t>
   </si>
   <si>
@@ -324,7 +315,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>71:59:34</t>
+    <t>72:00:27</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -1071,7 +1062,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1148,44 +1139,6 @@
       </c>
       <c r="L2" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1192,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1248,19 +1201,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
         <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s">
-        <v>72</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1269,7 +1222,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1277,7 +1230,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1286,19 +1239,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
         <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" t="s">
-        <v>78</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1307,7 +1260,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1315,31 +1268,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1347,31 +1300,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1385,7 +1338,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1428,7 +1381,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1437,19 +1390,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" t="s">
-        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1458,15 +1411,10 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1520,28 +1468,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1550,7 +1498,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:02:07 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:15:41</t>
+    <t>3930:16:06</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:48:19</t>
+    <t>69:48:44</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:48:19</t>
+    <t>92:48:44</t>
   </si>
   <si>
     <t>In progress</t>
@@ -135,166 +135,172 @@
     <t>team on the way</t>
   </si>
   <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
+    <t>PCM-20250421-00001074</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RIY2486</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>12111:39:47</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:13:03</t>
+  </si>
+  <si>
+    <t>site located in VIP Area and Generator switched off as per security request.</t>
+  </si>
+  <si>
+    <t>PCM-20250203-00001501</t>
+  </si>
+  <si>
+    <t>RIY2719</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:38:34</t>
+  </si>
+  <si>
+    <t>3241:23:16</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:30:04</t>
+  </si>
+  <si>
+    <t>Access Issue As Site located inside Wonder Garden.</t>
+  </si>
+  <si>
+    <t>PCM-20250529-00002138</t>
+  </si>
+  <si>
+    <t>RIY2903</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:27:00</t>
+  </si>
+  <si>
+    <t>479:34:50</t>
+  </si>
+  <si>
+    <t>2025-05-14 13:02:01</t>
+  </si>
+  <si>
+    <t>No BB</t>
+  </si>
+  <si>
+    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
+  </si>
+  <si>
+    <t>JED0190</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>HAL0947</t>
+  </si>
+  <si>
+    <t>Weak+Good</t>
+  </si>
+  <si>
+    <t>Zain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCM-20250215-00000830 </t>
+  </si>
+  <si>
+    <t>MKJD0649</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:32:14</t>
+  </si>
+  <si>
+    <t>2957:29:36</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:23:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
+  </si>
+  <si>
+    <t>PCM-20250611-00000037</t>
+  </si>
+  <si>
+    <t>JED2394</t>
+  </si>
+  <si>
+    <t>2025-06-11 00:19:59</t>
+  </si>
+  <si>
+    <t>184:41:51</t>
+  </si>
+  <si>
+    <t>2025-06-10 22:04:05</t>
+  </si>
+  <si>
+    <t>Site access issue  located in formula one  /Site under relocation</t>
+  </si>
+  <si>
+    <t>NO PCM</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TAF0156</t>
+  </si>
+  <si>
+    <t>2025-06-15 16:07:34</t>
+  </si>
+  <si>
+    <t>72:54:16</t>
+  </si>
+  <si>
+    <t>Access issue, located on commercial building, due to pending rent billing</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>JED0674</t>
+  </si>
+  <si>
+    <t>2025-06-15 18:30:01</t>
+  </si>
+  <si>
+    <t>70:31:49</t>
+  </si>
+  <si>
+    <t>25 m</t>
+  </si>
+  <si>
+    <t>PCM-20250531-00001907</t>
+  </si>
+  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>HAJ0155</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>PCM-20250421-00001074</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RIY2486</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>12111:39:21</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:13:03</t>
-  </si>
-  <si>
-    <t>site located in VIP Area and Generator switched off as per security request.</t>
-  </si>
-  <si>
-    <t>PCM-20250203-00001501</t>
-  </si>
-  <si>
-    <t>RIY2719</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:38:34</t>
-  </si>
-  <si>
-    <t>3241:22:50</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:30:04</t>
-  </si>
-  <si>
-    <t>Access Issue As Site located inside Wonder Garden.</t>
-  </si>
-  <si>
-    <t>PCM-20250529-00002138</t>
-  </si>
-  <si>
-    <t>RIY2903</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:27:00</t>
-  </si>
-  <si>
-    <t>479:34:24</t>
-  </si>
-  <si>
-    <t>2025-05-14 13:02:01</t>
-  </si>
-  <si>
-    <t>No BB</t>
-  </si>
-  <si>
-    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>HAL0947</t>
-  </si>
-  <si>
-    <t>Weak+Good</t>
-  </si>
-  <si>
-    <t>Zain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PCM-20250215-00000830 </t>
-  </si>
-  <si>
-    <t>MKJD0649</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:32:14</t>
-  </si>
-  <si>
-    <t>2957:29:10</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:23:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
-  </si>
-  <si>
-    <t>PCM-20250611-00000037</t>
-  </si>
-  <si>
-    <t>JED2394</t>
-  </si>
-  <si>
-    <t>2025-06-11 00:19:59</t>
-  </si>
-  <si>
-    <t>184:41:25</t>
-  </si>
-  <si>
-    <t>2025-06-10 22:04:05</t>
-  </si>
-  <si>
-    <t>Site access issue  located in formula one  /Site under relocation</t>
-  </si>
-  <si>
-    <t>NO PCM</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>TAF0156</t>
-  </si>
-  <si>
-    <t>2025-06-15 16:07:34</t>
-  </si>
-  <si>
-    <t>72:53:50</t>
-  </si>
-  <si>
-    <t>Access issue, located on commercial building, due to pending rent billing</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>JED0674</t>
-  </si>
-  <si>
-    <t>2025-06-15 18:30:01</t>
-  </si>
-  <si>
-    <t>70:31:23</t>
-  </si>
-  <si>
-    <t>25 m</t>
-  </si>
-  <si>
-    <t>PCM-20250531-00001907</t>
-  </si>
-  <si>
     <t>MAK0605</t>
   </si>
   <si>
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:28:09</t>
+    <t>431:28:35</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -303,6 +309,9 @@
     <t>Sectors are down due to TE issue and they are facing access issue. Access applied and waiting approval from court.</t>
   </si>
   <si>
+    <t>MAK0875</t>
+  </si>
+  <si>
     <t>PCM-20250615-00001771</t>
   </si>
   <si>
@@ -315,7 +324,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>72:00:27</t>
+    <t>72:00:53</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -858,31 +867,31 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
         <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>41</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -899,7 +908,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -942,28 +951,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -972,7 +981,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -980,28 +989,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
         <v>51</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1010,7 +1019,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1018,39 +1027,77 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
         <v>57</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>58</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" t="s">
         <v>60</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="L4" t="s">
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1108,13 +1155,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1132,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1192,7 +1239,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1201,19 +1248,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1222,7 +1269,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1230,7 +1277,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1239,19 +1286,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1260,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1268,31 +1315,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1300,31 +1347,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1338,7 +1385,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1381,28 +1428,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1411,10 +1458,15 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1468,28 +1520,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1498,7 +1550,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:03:20 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="107">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:16:06</t>
+    <t>3930:17:18</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:48:44</t>
+    <t>69:49:56</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:48:44</t>
+    <t>92:49:56</t>
   </si>
   <si>
     <t>In progress</t>
@@ -141,6 +141,15 @@
     <t>Good+In progress</t>
   </si>
   <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>HAJ0125</t>
+  </si>
+  <si>
+    <t>Haj Removal</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -153,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:39:47</t>
+    <t>12111:40:58</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -171,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3241:23:16</t>
+    <t>3241:24:27</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -189,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:34:50</t>
+    <t>479:36:01</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -228,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:29:36</t>
+    <t>2957:30:47</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -246,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:41:51</t>
+    <t>184:43:02</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -267,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:54:16</t>
+    <t>72:55:27</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -282,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:31:49</t>
+    <t>70:33:00</t>
   </si>
   <si>
     <t>25 m</t>
@@ -291,16 +300,13 @@
     <t>PCM-20250531-00001907</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>MAK0605</t>
   </si>
   <si>
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:28:35</t>
+    <t>431:29:46</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -324,7 +330,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>72:00:53</t>
+    <t>72:02:04</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -707,7 +713,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -897,6 +903,44 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -951,28 +995,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -981,7 +1025,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -989,28 +1033,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1019,7 +1063,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1027,37 +1071,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1074,7 +1118,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1092,7 +1136,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1155,13 +1199,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1179,13 +1223,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1283,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1248,19 +1292,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1269,7 +1313,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1277,7 +1321,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1286,19 +1330,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1307,7 +1351,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1315,31 +1359,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1347,31 +1391,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1428,28 +1472,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1458,7 +1502,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1466,7 +1510,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1520,28 +1564,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1550,7 +1594,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:03:50 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:17:18</t>
+    <t>3930:17:39</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:49:56</t>
+    <t>69:50:17</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:49:56</t>
+    <t>92:50:17</t>
   </si>
   <si>
     <t>In progress</t>
@@ -162,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:40:58</t>
+    <t>12111:41:29</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -180,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3241:24:27</t>
+    <t>3241:24:58</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -198,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:36:01</t>
+    <t>479:36:32</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -210,10 +210,10 @@
     <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
   </si>
   <si>
-    <t>JED0190</t>
-  </si>
-  <si>
-    <t>Good</t>
+    <t>JED0155</t>
+  </si>
+  <si>
+    <t>Good+Vandalized</t>
   </si>
   <si>
     <t>R3</t>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:30:47</t>
+    <t>2957:31:09</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:43:02</t>
+    <t>184:43:24</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:55:27</t>
+    <t>72:55:49</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:33:00</t>
+    <t>70:33:22</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:29:46</t>
+    <t>431:30:08</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -330,7 +330,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>72:02:04</t>
+    <t>72:02:26</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:05:05 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="106">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:17:39</t>
+    <t>3930:19:13</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:50:17</t>
+    <t>69:51:51</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:50:17</t>
+    <t>92:51:51</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,10 +144,10 @@
     <t>R5</t>
   </si>
   <si>
-    <t>HAJ0125</t>
-  </si>
-  <si>
-    <t>Haj Removal</t>
+    <t>HAJ0155</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
   <si>
     <t>PCM-20250421-00001074</t>
@@ -162,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:41:29</t>
+    <t>12111:42:52</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -180,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3241:24:58</t>
+    <t>3241:26:21</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -198,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:36:32</t>
+    <t>479:37:55</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -210,10 +210,7 @@
     <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
   </si>
   <si>
-    <t>JED0155</t>
-  </si>
-  <si>
-    <t>Good+Vandalized</t>
+    <t>JED0190</t>
   </si>
   <si>
     <t>R3</t>
@@ -237,7 +234,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:31:09</t>
+    <t>2957:32:41</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +252,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:43:24</t>
+    <t>184:44:56</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +273,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>72:55:49</t>
+    <t>72:57:21</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +288,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:33:22</t>
+    <t>70:34:54</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +303,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:30:08</t>
+    <t>431:31:40</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -330,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>72:02:26</t>
+    <t>72:03:58</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -1136,7 +1133,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1199,13 +1196,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1223,13 +1220,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>68</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1283,7 +1280,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1292,19 +1289,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>73</v>
-      </c>
-      <c r="H2" t="s">
-        <v>74</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1313,7 +1310,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1321,7 +1318,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1330,19 +1327,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
         <v>78</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>79</v>
-      </c>
-      <c r="H3" t="s">
-        <v>80</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1351,7 +1348,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1359,31 +1356,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
         <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
         <v>85</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1391,31 +1388,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
         <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>89</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" t="s">
         <v>90</v>
-      </c>
-      <c r="G5" t="s">
-        <v>91</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1472,7 +1469,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -1481,19 +1478,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
         <v>95</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>96</v>
-      </c>
-      <c r="H2" t="s">
-        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1502,7 +1499,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1510,7 +1507,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1564,28 +1561,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
         <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
         <v>103</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>104</v>
-      </c>
-      <c r="H2" t="s">
-        <v>105</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1594,7 +1591,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 5:08:02 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:19:13</t>
+    <t>3930:22:13</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:51:51</t>
+    <t>69:54:51</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:51:51</t>
+    <t>92:54:51</t>
   </si>
   <si>
     <t>In progress</t>
@@ -141,169 +141,166 @@
     <t>Good+In progress</t>
   </si>
   <si>
+    <t>PCM-20250421-00001074</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RIY2486</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>12111:45:53</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:13:03</t>
+  </si>
+  <si>
+    <t>site located in VIP Area and Generator switched off as per security request.</t>
+  </si>
+  <si>
+    <t>PCM-20250203-00001501</t>
+  </si>
+  <si>
+    <t>RIY2719</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:38:34</t>
+  </si>
+  <si>
+    <t>3241:29:22</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:30:04</t>
+  </si>
+  <si>
+    <t>Access Issue As Site located inside Wonder Garden.</t>
+  </si>
+  <si>
+    <t>PCM-20250529-00002138</t>
+  </si>
+  <si>
+    <t>RIY2903</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:27:00</t>
+  </si>
+  <si>
+    <t>479:40:56</t>
+  </si>
+  <si>
+    <t>2025-05-14 13:02:01</t>
+  </si>
+  <si>
+    <t>No BB</t>
+  </si>
+  <si>
+    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
+  </si>
+  <si>
+    <t>JED0190</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>HAL0947</t>
+  </si>
+  <si>
+    <t>Weak+Good</t>
+  </si>
+  <si>
+    <t>Zain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCM-20250215-00000830 </t>
+  </si>
+  <si>
+    <t>MKJD0649</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:32:14</t>
+  </si>
+  <si>
+    <t>2957:35:42</t>
+  </si>
+  <si>
+    <t>2025-02-15 11:23:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
+  </si>
+  <si>
+    <t>PCM-20250611-00000037</t>
+  </si>
+  <si>
+    <t>JED2394</t>
+  </si>
+  <si>
+    <t>2025-06-11 00:19:59</t>
+  </si>
+  <si>
+    <t>184:47:57</t>
+  </si>
+  <si>
+    <t>2025-06-10 22:04:05</t>
+  </si>
+  <si>
+    <t>Site access issue  located in formula one  /Site under relocation</t>
+  </si>
+  <si>
+    <t>NO PCM</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TAF0156</t>
+  </si>
+  <si>
+    <t>2025-06-15 16:07:34</t>
+  </si>
+  <si>
+    <t>73:00:22</t>
+  </si>
+  <si>
+    <t>Access issue, located on commercial building, due to pending rent billing</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>JED0674</t>
+  </si>
+  <si>
+    <t>2025-06-15 18:30:01</t>
+  </si>
+  <si>
+    <t>70:37:55</t>
+  </si>
+  <si>
+    <t>25 m</t>
+  </si>
+  <si>
+    <t>PCM-20250531-00001907</t>
+  </si>
+  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>HAJ0155</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>PCM-20250421-00001074</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RIY2486</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>12111:42:52</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:13:03</t>
-  </si>
-  <si>
-    <t>site located in VIP Area and Generator switched off as per security request.</t>
-  </si>
-  <si>
-    <t>PCM-20250203-00001501</t>
-  </si>
-  <si>
-    <t>RIY2719</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:38:34</t>
-  </si>
-  <si>
-    <t>3241:26:21</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:30:04</t>
-  </si>
-  <si>
-    <t>Access Issue As Site located inside Wonder Garden.</t>
-  </si>
-  <si>
-    <t>PCM-20250529-00002138</t>
-  </si>
-  <si>
-    <t>RIY2903</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:27:00</t>
-  </si>
-  <si>
-    <t>479:37:55</t>
-  </si>
-  <si>
-    <t>2025-05-14 13:02:01</t>
-  </si>
-  <si>
-    <t>No BB</t>
-  </si>
-  <si>
-    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
-  </si>
-  <si>
-    <t>JED0190</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>HAL0947</t>
-  </si>
-  <si>
-    <t>Weak+Good</t>
-  </si>
-  <si>
-    <t>Zain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PCM-20250215-00000830 </t>
-  </si>
-  <si>
-    <t>MKJD0649</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:32:14</t>
-  </si>
-  <si>
-    <t>2957:32:41</t>
-  </si>
-  <si>
-    <t>2025-02-15 11:23:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> site located in aramco area access issue need special permission</t>
-  </si>
-  <si>
-    <t>PCM-20250611-00000037</t>
-  </si>
-  <si>
-    <t>JED2394</t>
-  </si>
-  <si>
-    <t>2025-06-11 00:19:59</t>
-  </si>
-  <si>
-    <t>184:44:56</t>
-  </si>
-  <si>
-    <t>2025-06-10 22:04:05</t>
-  </si>
-  <si>
-    <t>Site access issue  located in formula one  /Site under relocation</t>
-  </si>
-  <si>
-    <t>NO PCM</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>TAF0156</t>
-  </si>
-  <si>
-    <t>2025-06-15 16:07:34</t>
-  </si>
-  <si>
-    <t>72:57:21</t>
-  </si>
-  <si>
-    <t>Access issue, located on commercial building, due to pending rent billing</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>JED0674</t>
-  </si>
-  <si>
-    <t>2025-06-15 18:30:01</t>
-  </si>
-  <si>
-    <t>70:34:54</t>
-  </si>
-  <si>
-    <t>25 m</t>
-  </si>
-  <si>
-    <t>PCM-20250531-00001907</t>
-  </si>
-  <si>
     <t>MAK0605</t>
   </si>
   <si>
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:31:40</t>
+    <t>431:34:41</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +324,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>72:03:58</t>
+    <t>72:06:59</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -710,7 +707,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -900,44 +897,6 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -992,28 +951,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1022,7 +981,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1030,28 +989,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1060,7 +1019,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1068,37 +1027,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1115,7 +1074,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1133,7 +1092,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1196,13 +1155,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1220,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1280,7 +1239,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1289,19 +1248,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
         <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" t="s">
-        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1310,7 +1269,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1318,7 +1277,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1327,19 +1286,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
         <v>77</v>
-      </c>
-      <c r="G3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1348,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1356,31 +1315,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1388,31 +1347,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1469,28 +1428,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>95</v>
-      </c>
-      <c r="H2" t="s">
-        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1499,7 +1458,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1507,7 +1466,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1561,28 +1520,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
         <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
         <v>102</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>103</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1591,7 +1550,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/18/2025, 6:01:27 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3930:22:13</t>
+    <t>3931:15:41</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>69:54:51</t>
+    <t>70:48:19</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>92:54:51</t>
+    <t>93:48:19</t>
   </si>
   <si>
     <t>In progress</t>
@@ -135,10 +135,13 @@
     <t>team on the way</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>USMD0705</t>
+  </si>
+  <si>
+    <t>Weak</t>
   </si>
   <si>
     <t>PCM-20250421-00001074</t>
@@ -153,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12111:45:53</t>
+    <t>12112:38:53</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -171,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3241:29:22</t>
+    <t>3242:22:22</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -189,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>479:40:56</t>
+    <t>480:33:56</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -228,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2957:35:42</t>
+    <t>2958:28:42</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -246,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>184:47:57</t>
+    <t>185:40:57</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -267,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>73:00:22</t>
+    <t>73:53:22</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -282,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>70:37:55</t>
+    <t>71:30:55</t>
   </si>
   <si>
     <t>25 m</t>
@@ -291,16 +294,13 @@
     <t>PCM-20250531-00001907</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>MAK0605</t>
   </si>
   <si>
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>431:34:41</t>
+    <t>432:27:41</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -324,7 +324,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>72:06:59</t>
+    <t>72:59:59</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -867,16 +867,16 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
@@ -888,13 +888,13 @@
         <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
@@ -951,28 +951,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -981,7 +981,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -989,28 +989,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1019,7 +1019,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1027,37 +1027,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1074,7 +1074,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1092,7 +1092,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1155,13 +1155,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1179,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1248,19 +1248,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1269,7 +1269,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1286,19 +1286,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1307,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1315,31 +1315,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1347,31 +1347,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1428,10 +1428,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 5:51:37 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="106">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3931:15:41</t>
+    <t>3943:05:39</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>70:48:19</t>
+    <t>82:38:17</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>93:48:19</t>
+    <t>105:38:17</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,6 +144,9 @@
     <t>Weak</t>
   </si>
   <si>
+    <t>JED0123</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -156,7 +159,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12112:38:53</t>
+    <t>12124:28:53</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +177,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3242:22:22</t>
+    <t>3254:12:22</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +195,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>480:33:56</t>
+    <t>492:23:56</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -231,7 +234,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2958:28:42</t>
+    <t>2970:18:42</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -249,7 +252,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>185:40:57</t>
+    <t>197:30:57</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -270,7 +273,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>73:53:22</t>
+    <t>85:43:22</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -285,7 +288,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>71:30:55</t>
+    <t>83:20:55</t>
   </si>
   <si>
     <t>25 m</t>
@@ -300,7 +303,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>432:27:41</t>
+    <t>444:17:41</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -324,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>72:59:59</t>
+    <t>84:49:59</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -707,7 +710,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -897,6 +900,44 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -951,28 +992,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -981,7 +1022,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -989,28 +1030,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1019,7 +1060,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1027,37 +1068,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1074,7 +1115,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1092,7 +1133,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1155,13 +1196,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1179,13 +1220,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1280,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1248,19 +1289,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1269,7 +1310,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1277,7 +1318,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1286,19 +1327,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1307,7 +1348,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1315,31 +1356,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1347,31 +1388,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1428,7 +1469,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1437,19 +1478,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1458,7 +1499,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1466,7 +1507,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1520,28 +1561,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1550,7 +1591,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 5:52:44 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="105">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3943:05:39</t>
+    <t>3943:06:11</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>82:38:17</t>
+    <t>82:38:49</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>105:38:17</t>
+    <t>105:38:49</t>
   </si>
   <si>
     <t>In progress</t>
@@ -159,7 +159,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12124:28:53</t>
+    <t>12124:29:52</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -177,7 +177,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3254:12:22</t>
+    <t>3254:13:21</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -195,7 +195,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>492:23:56</t>
+    <t>492:24:55</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -234,7 +234,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2970:18:42</t>
+    <t>2970:19:41</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -252,7 +252,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>197:30:57</t>
+    <t>197:31:56</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -273,7 +273,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>85:43:22</t>
+    <t>85:44:21</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -288,7 +288,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>83:20:55</t>
+    <t>83:21:54</t>
   </si>
   <si>
     <t>25 m</t>
@@ -303,7 +303,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>444:17:41</t>
+    <t>444:19:08</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -312,9 +312,6 @@
     <t>Sectors are down due to TE issue and they are facing access issue. Access applied and waiting approval from court.</t>
   </si>
   <si>
-    <t>MAK0875</t>
-  </si>
-  <si>
     <t>PCM-20250615-00001771</t>
   </si>
   <si>
@@ -327,7 +324,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>84:49:59</t>
+    <t>84:50:58</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -1505,9 +1502,42 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1561,28 +1591,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
         <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
         <v>102</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>103</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1591,7 +1621,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 7:43:40 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3943:06:11</t>
+    <t>3944:57:47</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>82:38:49</t>
+    <t>84:30:25</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>105:38:49</t>
+    <t>107:30:25</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,9 +144,6 @@
     <t>Weak</t>
   </si>
   <si>
-    <t>JED0123</t>
-  </si>
-  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -159,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12124:29:52</t>
+    <t>12126:21:27</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -177,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3254:13:21</t>
+    <t>3256:04:56</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -195,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>492:24:55</t>
+    <t>494:16:30</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -234,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2970:19:41</t>
+    <t>2972:11:16</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -252,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>197:31:56</t>
+    <t>199:23:31</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -273,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>85:44:21</t>
+    <t>87:35:56</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -288,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>83:21:54</t>
+    <t>85:13:29</t>
   </si>
   <si>
     <t>25 m</t>
@@ -303,7 +300,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>444:19:08</t>
+    <t>446:10:15</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -324,7 +321,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>84:50:58</t>
+    <t>86:42:33</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -707,7 +704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -897,44 +894,6 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -989,28 +948,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>48</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1019,7 +978,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1027,28 +986,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1057,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1065,37 +1024,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>59</v>
-      </c>
-      <c r="H4" t="s">
-        <v>60</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" t="s">
         <v>61</v>
-      </c>
-      <c r="K4" t="s">
-        <v>62</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1112,7 +1071,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1130,7 +1089,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1193,13 +1152,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1217,13 +1176,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>67</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1236,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1286,19 +1245,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>72</v>
-      </c>
-      <c r="H2" t="s">
-        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1307,7 +1266,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1315,7 +1274,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1324,19 +1283,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>78</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1345,7 +1304,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1353,31 +1312,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" t="s">
         <v>84</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1385,31 +1344,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
         <v>87</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
         <v>89</v>
-      </c>
-      <c r="G5" t="s">
-        <v>90</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1466,7 +1425,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1475,19 +1434,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>95</v>
-      </c>
-      <c r="H2" t="s">
-        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1496,7 +1455,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1513,7 +1472,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1591,28 +1550,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>101</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>102</v>
-      </c>
-      <c r="H2" t="s">
-        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1621,7 +1580,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 7:44:40 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="105">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3944:57:47</t>
+    <t>3944:58:47</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>84:30:25</t>
+    <t>84:31:25</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>107:30:25</t>
+    <t>107:31:25</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,6 +144,12 @@
     <t>Weak</t>
   </si>
   <si>
+    <t>HAJ0155</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -156,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12126:21:27</t>
+    <t>12126:22:26</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3256:04:56</t>
+    <t>3256:05:55</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>494:16:30</t>
+    <t>494:17:29</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -207,9 +213,6 @@
     <t>JED0190</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -231,7 +234,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2972:11:16</t>
+    <t>2972:12:15</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -249,7 +252,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>199:23:31</t>
+    <t>199:24:30</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -270,7 +273,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>87:35:56</t>
+    <t>87:36:55</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -285,7 +288,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>85:13:29</t>
+    <t>85:14:28</t>
   </si>
   <si>
     <t>25 m</t>
@@ -300,7 +303,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>446:10:15</t>
+    <t>446:11:14</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -321,7 +324,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>86:42:33</t>
+    <t>86:43:32</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -704,7 +707,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -894,6 +897,44 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -948,28 +989,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -978,7 +1019,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -986,28 +1027,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1016,7 +1057,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1024,37 +1065,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1071,7 +1112,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1089,7 +1130,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1152,13 +1193,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1176,13 +1217,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1277,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1245,19 +1286,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1266,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1274,7 +1315,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1283,19 +1324,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1304,7 +1345,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1312,31 +1353,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1344,31 +1385,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1425,7 +1466,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1434,19 +1475,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1455,7 +1496,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1472,7 +1513,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1550,28 +1591,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1580,7 +1621,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 8:19:08 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3944:58:47</t>
+    <t>3945:33:21</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>84:31:25</t>
+    <t>85:05:59</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>107:31:25</t>
+    <t>108:05:59</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,75 +144,72 @@
     <t>Weak</t>
   </si>
   <si>
-    <t>HAJ0155</t>
+    <t>PCM-20250421-00001074</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RIY2486</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>12126:57:02</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:13:03</t>
+  </si>
+  <si>
+    <t>site located in VIP Area and Generator switched off as per security request.</t>
+  </si>
+  <si>
+    <t>PCM-20250203-00001501</t>
+  </si>
+  <si>
+    <t>RIY2719</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:38:34</t>
+  </si>
+  <si>
+    <t>3256:40:31</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:30:04</t>
+  </si>
+  <si>
+    <t>Access Issue As Site located inside Wonder Garden.</t>
+  </si>
+  <si>
+    <t>PCM-20250529-00002138</t>
+  </si>
+  <si>
+    <t>RIY2903</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:27:00</t>
+  </si>
+  <si>
+    <t>494:52:05</t>
+  </si>
+  <si>
+    <t>2025-05-14 13:02:01</t>
+  </si>
+  <si>
+    <t>No BB</t>
+  </si>
+  <si>
+    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
+  </si>
+  <si>
+    <t>JED0190</t>
   </si>
   <si>
     <t>Good</t>
   </si>
   <si>
-    <t>PCM-20250421-00001074</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RIY2486</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>12126:22:26</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:13:03</t>
-  </si>
-  <si>
-    <t>site located in VIP Area and Generator switched off as per security request.</t>
-  </si>
-  <si>
-    <t>PCM-20250203-00001501</t>
-  </si>
-  <si>
-    <t>RIY2719</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:38:34</t>
-  </si>
-  <si>
-    <t>3256:05:55</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:30:04</t>
-  </si>
-  <si>
-    <t>Access Issue As Site located inside Wonder Garden.</t>
-  </si>
-  <si>
-    <t>PCM-20250529-00002138</t>
-  </si>
-  <si>
-    <t>RIY2903</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:27:00</t>
-  </si>
-  <si>
-    <t>494:17:29</t>
-  </si>
-  <si>
-    <t>2025-05-14 13:02:01</t>
-  </si>
-  <si>
-    <t>No BB</t>
-  </si>
-  <si>
-    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
-  </si>
-  <si>
-    <t>JED0190</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -234,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2972:12:15</t>
+    <t>2972:46:51</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -252,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>199:24:30</t>
+    <t>199:59:06</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -273,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>87:36:55</t>
+    <t>88:11:31</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -288,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>85:14:28</t>
+    <t>85:49:04</t>
   </si>
   <si>
     <t>25 m</t>
@@ -303,7 +300,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>446:11:14</t>
+    <t>446:45:50</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -324,7 +321,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>86:43:32</t>
+    <t>87:18:08</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -707,7 +704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -897,44 +894,6 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -989,28 +948,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>49</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1019,7 +978,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1027,28 +986,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
         <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" t="s">
-        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1057,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1065,37 +1024,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
         <v>59</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>61</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1112,7 +1071,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1130,7 +1089,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1193,13 +1152,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1217,13 +1176,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>67</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1236,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1286,19 +1245,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>72</v>
-      </c>
-      <c r="H2" t="s">
-        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1307,7 +1266,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1315,7 +1274,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1324,19 +1283,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>78</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1345,7 +1304,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1353,31 +1312,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" t="s">
         <v>84</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1385,31 +1344,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
         <v>87</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
         <v>89</v>
-      </c>
-      <c r="G5" t="s">
-        <v>90</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1466,7 +1425,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1475,19 +1434,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>95</v>
-      </c>
-      <c r="H2" t="s">
-        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1496,7 +1455,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1513,7 +1472,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1591,28 +1550,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>101</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>102</v>
-      </c>
-      <c r="H2" t="s">
-        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1621,7 +1580,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 9:13:13 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="108">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3945:33:21</t>
+    <t>3946:27:15</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>85:05:59</t>
+    <t>85:59:53</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>108:05:59</t>
+    <t>108:59:53</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,6 +144,18 @@
     <t>Weak</t>
   </si>
   <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>2025-06-19 09:13:02</t>
+  </si>
+  <si>
+    <t>0:00:00</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -156,7 +168,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12126:57:02</t>
+    <t>12127:49:56</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +186,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3256:40:31</t>
+    <t>3257:33:25</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +204,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>494:52:05</t>
+    <t>495:44:59</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -231,7 +243,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2972:46:51</t>
+    <t>2973:39:45</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -249,7 +261,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>199:59:06</t>
+    <t>200:52:00</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -270,7 +282,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>88:11:31</t>
+    <t>89:04:25</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -285,7 +297,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>85:49:04</t>
+    <t>86:41:58</t>
   </si>
   <si>
     <t>25 m</t>
@@ -300,7 +312,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>446:45:50</t>
+    <t>447:38:44</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -321,7 +333,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>87:18:08</t>
+    <t>88:11:02</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -704,7 +716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -894,6 +906,44 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -948,28 +998,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -978,7 +1028,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -986,28 +1036,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1016,7 +1066,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1024,37 +1074,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1071,7 +1121,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1089,7 +1139,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1152,13 +1202,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1176,13 +1226,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1286,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1245,19 +1295,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1266,7 +1316,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1274,7 +1324,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1283,19 +1333,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1304,7 +1354,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1312,31 +1362,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1344,31 +1394,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1425,7 +1475,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1434,19 +1484,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1455,7 +1505,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1472,7 +1522,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1550,28 +1600,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1580,7 +1630,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 9:13:27 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3946:27:15</t>
+    <t>3946:27:33</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>85:59:53</t>
+    <t>86:00:11</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>108:59:53</t>
+    <t>109:00:11</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,18 +144,6 @@
     <t>Weak</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>2025-06-19 09:13:02</t>
-  </si>
-  <si>
-    <t>0:00:00</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
-  </si>
-  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -168,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12127:49:56</t>
+    <t>12127:51:14</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -186,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3257:33:25</t>
+    <t>3257:34:43</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -204,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>495:44:59</t>
+    <t>495:46:17</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -243,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2973:39:45</t>
+    <t>2973:41:03</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -261,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>200:52:00</t>
+    <t>200:53:18</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -282,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>89:04:25</t>
+    <t>89:05:43</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -297,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>86:41:58</t>
+    <t>86:43:16</t>
   </si>
   <si>
     <t>25 m</t>
@@ -312,7 +300,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>447:38:44</t>
+    <t>447:40:02</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -333,7 +321,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>88:11:02</t>
+    <t>88:12:20</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -716,7 +704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -906,44 +894,6 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -998,28 +948,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1028,7 +978,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1036,28 +986,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1066,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1074,37 +1024,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1121,7 +1071,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1139,7 +1089,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1202,13 +1152,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1226,13 +1176,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1286,7 +1236,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1295,19 +1245,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1316,7 +1266,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1324,7 +1274,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1333,19 +1283,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1354,7 +1304,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1362,31 +1312,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1394,31 +1344,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1475,7 +1425,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1484,19 +1434,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1505,7 +1455,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1522,7 +1472,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1600,28 +1550,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1630,7 +1580,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 9:15:20 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="105">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3946:27:33</t>
+    <t>3946:29:17</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>86:00:11</t>
+    <t>86:01:55</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>109:00:11</t>
+    <t>109:01:55</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,6 +144,9 @@
     <t>Weak</t>
   </si>
   <si>
+    <t>JED0124</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -156,7 +159,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12127:51:14</t>
+    <t>12127:52:58</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +177,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3257:34:43</t>
+    <t>3257:36:27</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +195,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>495:46:17</t>
+    <t>495:48:01</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -231,7 +234,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2973:41:03</t>
+    <t>2973:42:47</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -249,7 +252,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>200:53:18</t>
+    <t>200:55:02</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -270,7 +273,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>89:05:43</t>
+    <t>89:07:27</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -285,7 +288,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>86:43:16</t>
+    <t>86:45:00</t>
   </si>
   <si>
     <t>25 m</t>
@@ -300,7 +303,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>447:40:02</t>
+    <t>447:41:46</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -321,7 +324,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>88:12:20</t>
+    <t>88:14:04</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -704,7 +707,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -894,6 +897,44 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -948,28 +989,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -978,7 +1019,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -986,28 +1027,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1016,7 +1057,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1024,37 +1065,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1071,7 +1112,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1089,7 +1130,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1152,13 +1193,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1176,13 +1217,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1277,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1245,19 +1286,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1266,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1274,7 +1315,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1283,19 +1324,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1304,7 +1345,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1312,31 +1353,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1344,31 +1385,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1425,7 +1466,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1434,19 +1475,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1455,7 +1496,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1472,7 +1513,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1550,28 +1591,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1580,7 +1621,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 9:39:05 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3946:29:17</t>
+    <t>3946:53:15</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>86:01:55</t>
+    <t>86:25:53</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>109:01:55</t>
+    <t>109:25:53</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,9 +144,6 @@
     <t>Weak</t>
   </si>
   <si>
-    <t>JED0124</t>
-  </si>
-  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -159,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12127:52:58</t>
+    <t>12128:16:53</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -177,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3257:36:27</t>
+    <t>3258:00:22</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -195,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>495:48:01</t>
+    <t>496:11:56</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -234,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2973:42:47</t>
+    <t>2974:06:42</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -252,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>200:55:02</t>
+    <t>201:18:57</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -273,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>89:07:27</t>
+    <t>89:31:22</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -288,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>86:45:00</t>
+    <t>87:08:55</t>
   </si>
   <si>
     <t>25 m</t>
@@ -303,7 +300,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>447:41:46</t>
+    <t>448:05:41</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -324,7 +321,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>88:14:04</t>
+    <t>88:37:59</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -707,7 +704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -897,44 +894,6 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -989,28 +948,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>48</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1019,7 +978,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1027,28 +986,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1057,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1065,37 +1024,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>59</v>
-      </c>
-      <c r="H4" t="s">
-        <v>60</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" t="s">
         <v>61</v>
-      </c>
-      <c r="K4" t="s">
-        <v>62</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1112,7 +1071,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1130,7 +1089,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1193,13 +1152,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1217,13 +1176,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>67</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1236,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1286,19 +1245,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>72</v>
-      </c>
-      <c r="H2" t="s">
-        <v>73</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1307,7 +1266,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1315,7 +1274,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1324,19 +1283,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>78</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1345,7 +1304,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1353,31 +1312,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" t="s">
         <v>84</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1385,31 +1344,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
         <v>87</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
         <v>89</v>
-      </c>
-      <c r="G5" t="s">
-        <v>90</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1466,7 +1425,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1475,19 +1434,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>95</v>
-      </c>
-      <c r="H2" t="s">
-        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1496,7 +1455,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1513,7 +1472,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1591,28 +1550,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>101</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>102</v>
-      </c>
-      <c r="H2" t="s">
-        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1621,7 +1580,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 10:14:20 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="104">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3946:53:15</t>
+    <t>3947:28:24</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>86:25:53</t>
+    <t>87:01:02</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>109:25:53</t>
+    <t>110:01:02</t>
   </si>
   <si>
     <t>In progress</t>
@@ -156,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12128:16:53</t>
+    <t>12128:52:02</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3258:00:22</t>
+    <t>3258:35:31</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>496:11:56</t>
+    <t>496:47:05</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -231,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2974:06:42</t>
+    <t>2974:41:51</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -249,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>201:18:57</t>
+    <t>201:54:06</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -270,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>89:31:22</t>
+    <t>90:06:31</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -285,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>87:08:55</t>
+    <t>87:44:04</t>
   </si>
   <si>
     <t>25 m</t>
@@ -300,7 +300,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>448:05:41</t>
+    <t>448:40:50</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -321,7 +321,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>88:37:59</t>
+    <t>89:13:08</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -704,7 +704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -895,6 +895,44 @@
       </c>
       <c r="L5" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 10:14:45 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="106">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3947:28:24</t>
+    <t>3947:28:51</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>87:01:02</t>
+    <t>87:01:29</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>110:01:02</t>
+    <t>110:01:29</t>
   </si>
   <si>
     <t>In progress</t>
@@ -156,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12128:52:02</t>
+    <t>12128:52:32</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3258:35:31</t>
+    <t>3258:36:01</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>496:47:05</t>
+    <t>496:47:35</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -210,6 +210,12 @@
     <t>Good</t>
   </si>
   <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
@@ -231,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2974:41:51</t>
+    <t>2974:42:21</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -249,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>201:54:06</t>
+    <t>201:54:36</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -270,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>90:06:31</t>
+    <t>90:07:01</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -285,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>87:44:04</t>
+    <t>87:44:34</t>
   </si>
   <si>
     <t>25 m</t>
@@ -300,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>448:40:50</t>
+    <t>448:41:20</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -321,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>89:13:08</t>
+    <t>89:13:38</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -704,7 +710,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -895,44 +901,6 @@
       </c>
       <c r="L5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +911,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1133,6 +1101,44 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1190,13 +1196,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1214,13 +1220,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1274,7 +1280,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1283,19 +1289,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1304,7 +1310,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1321,19 +1327,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1342,7 +1348,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1350,31 +1356,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1382,31 +1388,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1463,7 +1469,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1472,19 +1478,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1493,7 +1499,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1510,7 +1516,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1588,28 +1594,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1618,7 +1624,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 10:20:47 AM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3947:28:51</t>
+    <t>3947:35:00</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>87:01:29</t>
+    <t>87:07:38</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>110:01:29</t>
+    <t>110:07:38</t>
   </si>
   <si>
     <t>In progress</t>
@@ -156,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12128:52:32</t>
+    <t>12128:58:41</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3258:36:01</t>
+    <t>3258:42:10</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>496:47:35</t>
+    <t>496:53:44</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2974:42:21</t>
+    <t>2974:48:30</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>201:54:36</t>
+    <t>202:00:45</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>90:07:01</t>
+    <t>90:13:10</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>87:44:34</t>
+    <t>87:50:43</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>448:41:20</t>
+    <t>448:47:29</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>89:13:38</t>
+    <t>89:19:47</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 1:56:17 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="106">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3947:35:00</t>
+    <t>3951:10:15</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>87:07:38</t>
+    <t>90:42:53</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>110:07:38</t>
+    <t>113:42:53</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,6 +144,12 @@
     <t>Weak</t>
   </si>
   <si>
+    <t>JED0125</t>
+  </si>
+  <si>
+    <t>Good+In progress</t>
+  </si>
+  <si>
     <t>PCM-20250421-00001074</t>
   </si>
   <si>
@@ -156,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12128:58:41</t>
+    <t>12132:33:56</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3258:42:10</t>
+    <t>3262:17:25</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>496:53:44</t>
+    <t>500:28:59</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -210,12 +216,6 @@
     <t>Good</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2974:48:30</t>
+    <t>2978:23:45</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>202:00:45</t>
+    <t>205:36:00</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>90:13:10</t>
+    <t>93:48:25</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>87:50:43</t>
+    <t>91:25:58</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>448:47:29</t>
+    <t>452:22:44</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>89:19:47</t>
+    <t>92:55:02</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -710,7 +710,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -900,6 +900,44 @@
         <v>38</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -954,28 +992,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -984,7 +1022,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -992,28 +1030,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1022,7 +1060,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1030,37 +1068,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1077,7 +1115,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1095,7 +1133,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1115,7 +1153,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1133,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 2:28:58 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3951:10:15</t>
+    <t>3951:43:13</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>90:42:53</t>
+    <t>91:15:51</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>113:42:53</t>
+    <t>114:15:51</t>
   </si>
   <si>
     <t>In progress</t>
@@ -162,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12132:33:56</t>
+    <t>12133:06:53</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -180,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3262:17:25</t>
+    <t>3262:50:22</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -198,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>500:28:59</t>
+    <t>501:01:56</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2978:23:45</t>
+    <t>2978:56:42</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>205:36:00</t>
+    <t>206:08:57</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>93:48:25</t>
+    <t>94:21:22</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>91:25:58</t>
+    <t>91:58:55</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>452:22:44</t>
+    <t>452:55:41</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>92:55:02</t>
+    <t>93:27:59</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 2:29:05 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3951:43:13</t>
+    <t>3951:43:18</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>91:15:51</t>
+    <t>91:15:56</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>114:15:51</t>
+    <t>114:15:56</t>
   </si>
   <si>
     <t>In progress</t>
@@ -162,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12133:06:53</t>
+    <t>12133:06:59</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -180,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3262:50:22</t>
+    <t>3262:50:28</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -198,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>501:01:56</t>
+    <t>501:02:02</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2978:56:42</t>
+    <t>2978:56:48</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>206:08:57</t>
+    <t>206:09:03</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>94:21:22</t>
+    <t>94:21:28</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>91:58:55</t>
+    <t>91:59:01</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>452:55:41</t>
+    <t>452:55:47</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>93:27:59</t>
+    <t>93:28:05</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 3:13:14 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="106">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3951:43:18</t>
+    <t>3952:27:18</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>91:15:56</t>
+    <t>91:59:56</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>114:15:56</t>
+    <t>114:59:56</t>
   </si>
   <si>
     <t>In progress</t>
@@ -162,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12133:06:59</t>
+    <t>12133:50:58</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -180,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3262:50:28</t>
+    <t>3263:34:27</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -198,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>501:02:02</t>
+    <t>501:46:01</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2978:56:48</t>
+    <t>2979:40:47</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>206:09:03</t>
+    <t>206:53:02</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>94:21:28</t>
+    <t>95:05:27</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>91:59:01</t>
+    <t>92:43:00</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>452:55:47</t>
+    <t>453:39:46</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>93:28:05</t>
+    <t>94:12:04</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -710,7 +710,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -939,6 +939,44 @@
       </c>
       <c r="L6" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 3:13:35 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="106">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3952:27:18</t>
+    <t>3952:27:48</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>91:59:56</t>
+    <t>92:00:26</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>114:59:56</t>
+    <t>115:00:26</t>
   </si>
   <si>
     <t>In progress</t>
@@ -162,7 +162,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12133:50:58</t>
+    <t>12133:51:26</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -180,7 +180,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3263:34:27</t>
+    <t>3263:34:55</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -198,7 +198,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>501:46:01</t>
+    <t>501:46:29</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2979:40:47</t>
+    <t>2979:41:15</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>206:53:02</t>
+    <t>206:53:30</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>95:05:27</t>
+    <t>95:05:55</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>92:43:00</t>
+    <t>92:43:28</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>453:39:46</t>
+    <t>453:40:14</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>94:12:04</t>
+    <t>94:12:32</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -710,7 +710,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -939,44 +939,6 @@
       </c>
       <c r="L6" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 10:15:32 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3952:27:48</t>
+    <t>3959:29:33</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>92:00:26</t>
+    <t>99:02:11</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>115:00:26</t>
+    <t>122:02:11</t>
   </si>
   <si>
     <t>In progress</t>
@@ -144,78 +144,78 @@
     <t>Weak</t>
   </si>
   <si>
+    <t>PCM-20250421-00001074</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RIY2486</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:22:03</t>
+  </si>
+  <si>
+    <t>12139:22:43</t>
+  </si>
+  <si>
+    <t>2024-01-31 01:13:03</t>
+  </si>
+  <si>
+    <t>site located in VIP Area and Generator switched off as per security request.</t>
+  </si>
+  <si>
+    <t>PCM-20250203-00001501</t>
+  </si>
+  <si>
+    <t>RIY2719</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:38:34</t>
+  </si>
+  <si>
+    <t>3269:06:12</t>
+  </si>
+  <si>
+    <t>2025-02-03 15:30:04</t>
+  </si>
+  <si>
+    <t>Access Issue As Site located inside Wonder Garden.</t>
+  </si>
+  <si>
+    <t>PCM-20250529-00002138</t>
+  </si>
+  <si>
+    <t>RIY2903</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:27:00</t>
+  </si>
+  <si>
+    <t>507:17:46</t>
+  </si>
+  <si>
+    <t>2025-05-14 13:02:01</t>
+  </si>
+  <si>
+    <t>No BB</t>
+  </si>
+  <si>
+    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
+  </si>
+  <si>
+    <t>JED0190</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
     <t>JED0125</t>
   </si>
   <si>
     <t>Good+In progress</t>
   </si>
   <si>
-    <t>PCM-20250421-00001074</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RIY2486</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:22:03</t>
-  </si>
-  <si>
-    <t>12133:51:26</t>
-  </si>
-  <si>
-    <t>2024-01-31 01:13:03</t>
-  </si>
-  <si>
-    <t>site located in VIP Area and Generator switched off as per security request.</t>
-  </si>
-  <si>
-    <t>PCM-20250203-00001501</t>
-  </si>
-  <si>
-    <t>RIY2719</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:38:34</t>
-  </si>
-  <si>
-    <t>3263:34:55</t>
-  </si>
-  <si>
-    <t>2025-02-03 15:30:04</t>
-  </si>
-  <si>
-    <t>Access Issue As Site located inside Wonder Garden.</t>
-  </si>
-  <si>
-    <t>PCM-20250529-00002138</t>
-  </si>
-  <si>
-    <t>RIY2903</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:27:00</t>
-  </si>
-  <si>
-    <t>501:46:29</t>
-  </si>
-  <si>
-    <t>2025-05-14 13:02:01</t>
-  </si>
-  <si>
-    <t>No BB</t>
-  </si>
-  <si>
-    <t>We face access Issue Due Boulevard Gate , STC Owner , access PG</t>
-  </si>
-  <si>
-    <t>JED0190</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -237,7 +237,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2979:41:15</t>
+    <t>2985:12:32</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +255,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>206:53:30</t>
+    <t>212:24:47</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +276,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>95:05:55</t>
+    <t>100:37:12</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +291,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>92:43:28</t>
+    <t>98:14:45</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +306,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>453:40:14</t>
+    <t>459:11:31</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +327,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>94:12:32</t>
+    <t>99:43:49</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -914,7 +914,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -932,7 +932,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>
@@ -992,28 +992,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>49</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1022,7 +1022,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1030,28 +1030,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
         <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" t="s">
-        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1060,7 +1060,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1068,37 +1068,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
         <v>59</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>61</v>
       </c>
       <c r="I4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1115,7 +1115,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1133,7 +1133,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -1153,7 +1153,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1171,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Update Active_Outages.xlsx - 6/19/2025, 10:15:59 PM
</commit_message>
<xml_diff>
--- a/Active_Outages.xlsx
+++ b/Active_Outages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
   <si>
     <t>PCM</t>
   </si>
@@ -72,7 +72,7 @@
     <t>2025-01-05 22:45:44</t>
   </si>
   <si>
-    <t>3959:29:33</t>
+    <t>3959:29:56</t>
   </si>
   <si>
     <t>2025-01-05 22:38:30</t>
@@ -99,7 +99,7 @@
     <t>2025-06-15 19:13:06</t>
   </si>
   <si>
-    <t>99:02:11</t>
+    <t>99:02:34</t>
   </si>
   <si>
     <t>SCECO</t>
@@ -126,7 +126,7 @@
     <t>2025-06-14 20:13:06</t>
   </si>
   <si>
-    <t>122:02:11</t>
+    <t>122:02:34</t>
   </si>
   <si>
     <t>In progress</t>
@@ -156,7 +156,7 @@
     <t>2024-01-31 01:22:03</t>
   </si>
   <si>
-    <t>12139:22:43</t>
+    <t>12140:53:44</t>
   </si>
   <si>
     <t>2024-01-31 01:13:03</t>
@@ -174,7 +174,7 @@
     <t>2025-02-03 15:38:34</t>
   </si>
   <si>
-    <t>3269:06:12</t>
+    <t>3270:37:13</t>
   </si>
   <si>
     <t>2025-02-03 15:30:04</t>
@@ -192,7 +192,7 @@
     <t>2025-05-29 17:27:00</t>
   </si>
   <si>
-    <t>507:17:46</t>
+    <t>508:48:47</t>
   </si>
   <si>
     <t>2025-05-14 13:02:01</t>
@@ -210,12 +210,6 @@
     <t>Good</t>
   </si>
   <si>
-    <t>JED0125</t>
-  </si>
-  <si>
-    <t>Good+In progress</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -237,7 +231,7 @@
     <t>2025-02-15 11:32:14</t>
   </si>
   <si>
-    <t>2985:12:32</t>
+    <t>2986:43:26</t>
   </si>
   <si>
     <t>2025-02-15 11:23:40</t>
@@ -255,7 +249,7 @@
     <t>2025-06-11 00:19:59</t>
   </si>
   <si>
-    <t>212:24:47</t>
+    <t>213:55:41</t>
   </si>
   <si>
     <t>2025-06-10 22:04:05</t>
@@ -276,7 +270,7 @@
     <t>2025-06-15 16:07:34</t>
   </si>
   <si>
-    <t>100:37:12</t>
+    <t>102:08:06</t>
   </si>
   <si>
     <t>Access issue, located on commercial building, due to pending rent billing</t>
@@ -291,7 +285,7 @@
     <t>2025-06-15 18:30:01</t>
   </si>
   <si>
-    <t>98:14:45</t>
+    <t>99:45:39</t>
   </si>
   <si>
     <t>25 m</t>
@@ -306,7 +300,7 @@
     <t>2025-05-31 17:33:15</t>
   </si>
   <si>
-    <t>459:11:31</t>
+    <t>460:42:25</t>
   </si>
   <si>
     <t>2025-05-30 17:59:05</t>
@@ -327,7 +321,7 @@
     <t>2025-06-15 17:00:57</t>
   </si>
   <si>
-    <t>99:43:49</t>
+    <t>101:14:43</t>
   </si>
   <si>
     <t>2025-06-15 17:18:01</t>
@@ -1153,7 +1147,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1171,7 +1165,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>
@@ -1234,13 +1228,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1258,13 +1252,13 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1318,7 +1312,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -1327,19 +1321,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" t="s">
-        <v>74</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1348,7 +1342,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1356,7 +1350,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -1365,19 +1359,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s">
         <v>78</v>
-      </c>
-      <c r="G3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" t="s">
-        <v>80</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1386,7 +1380,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1394,31 +1388,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1426,31 +1420,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1507,7 +1501,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -1516,19 +1510,19 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
         <v>95</v>
-      </c>
-      <c r="G2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" t="s">
-        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1537,7 +1531,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -1554,7 +1548,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1632,28 +1626,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" t="s">
         <v>102</v>
-      </c>
-      <c r="G2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1662,7 +1656,7 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>

</xml_diff>